<commit_message>
Updated Streamlit app - rewritten code and fixes
</commit_message>
<xml_diff>
--- a/Apartment_Progress_Weighted-Progress_App_ITowerAvg_AppView_v5.xlsx
+++ b/Apartment_Progress_Weighted-Progress_App_ITowerAvg_AppView_v5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tower_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD55AB2A-A90E-4F25-A449-A1BD05A60FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA83351-3F76-490F-93EF-87BCB41D6F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1929,20 +1929,35 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="22" fontId="16" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1953,35 +1968,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2010,6 +2001,15 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2019,35 +2019,35 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="16" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -11048,14 +11048,14 @@
       </c>
       <c r="B7" s="27">
         <f>IFERROR(INDEX('Apartment Progress'!$O$4:$O$179, MATCH($B$3, 'Apartment Progress'!$A$4:$A$179, 0)), "")</f>
-        <v>0.82600000000000018</v>
+        <v>0.8480000000000002</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="33">
         <f>'Apartment Progress'!O3</f>
-        <v>0.65428118181818196</v>
+        <v>0.67356022727272735</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -11367,9 +11367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P209"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="G1" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11432,13 +11432,13 @@
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="161">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="D2" s="161">
         <v>0.15</v>
       </c>
       <c r="E2" s="161">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="F2" s="161">
         <v>0.1</v>
@@ -11456,13 +11456,13 @@
         <v>0.02</v>
       </c>
       <c r="K2" s="161">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="L2" s="161">
         <v>0.01</v>
       </c>
       <c r="M2" s="161">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="N2" s="161">
         <v>0.01</v>
@@ -11525,7 +11525,7 @@
       </c>
       <c r="O3" s="16">
         <f t="shared" ref="O3:O34" si="0">SUMPRODUCT(C3:N3, C$2:N$2)</f>
-        <v>0.65428118181818196</v>
+        <v>0.67356022727272735</v>
       </c>
       <c r="P3" s="21"/>
     </row>
@@ -11584,7 +11584,7 @@
       </c>
       <c r="O4" s="16">
         <f t="shared" si="0"/>
-        <v>0.89173333333333338</v>
+        <v>0.9137333333333334</v>
       </c>
       <c r="P4" s="14"/>
     </row>
@@ -11641,7 +11641,7 @@
       </c>
       <c r="O5" s="23">
         <f t="shared" si="0"/>
-        <v>0.82600000000000018</v>
+        <v>0.8480000000000002</v>
       </c>
       <c r="P5" s="7"/>
     </row>
@@ -11698,7 +11698,7 @@
       </c>
       <c r="O6" s="23">
         <f t="shared" si="0"/>
-        <v>0.86950000000000005</v>
+        <v>0.89150000000000007</v>
       </c>
       <c r="P6" s="8"/>
     </row>
@@ -11755,7 +11755,7 @@
       </c>
       <c r="O7" s="23">
         <f t="shared" si="0"/>
-        <v>0.90100000000000013</v>
+        <v>0.92300000000000015</v>
       </c>
       <c r="P7" s="8"/>
     </row>
@@ -11812,7 +11812,7 @@
       </c>
       <c r="O8" s="23">
         <f t="shared" si="0"/>
-        <v>0.85050000000000014</v>
+        <v>0.87250000000000016</v>
       </c>
       <c r="P8" s="8"/>
     </row>
@@ -11869,7 +11869,7 @@
       </c>
       <c r="O9" s="23">
         <f t="shared" si="0"/>
-        <v>0.87950000000000006</v>
+        <v>0.90150000000000008</v>
       </c>
       <c r="P9" s="8"/>
     </row>
@@ -11926,7 +11926,7 @@
       </c>
       <c r="O10" s="23">
         <f t="shared" si="0"/>
-        <v>0.90850000000000009</v>
+        <v>0.9305000000000001</v>
       </c>
       <c r="P10" s="8"/>
     </row>
@@ -11983,7 +11983,7 @@
       </c>
       <c r="O11" s="23">
         <f t="shared" si="0"/>
-        <v>0.90100000000000013</v>
+        <v>0.92300000000000015</v>
       </c>
       <c r="P11" s="8"/>
     </row>
@@ -12040,7 +12040,7 @@
       </c>
       <c r="O12" s="23">
         <f t="shared" si="0"/>
-        <v>0.91850000000000009</v>
+        <v>0.94050000000000011</v>
       </c>
       <c r="P12" s="8"/>
     </row>
@@ -12097,7 +12097,7 @@
       </c>
       <c r="O13" s="23">
         <f t="shared" si="0"/>
-        <v>0.90100000000000013</v>
+        <v>0.92300000000000015</v>
       </c>
       <c r="P13" s="8"/>
     </row>
@@ -12154,7 +12154,7 @@
       </c>
       <c r="O14" s="23">
         <f t="shared" si="0"/>
-        <v>0.91100000000000003</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="P14" s="8"/>
     </row>
@@ -12211,7 +12211,7 @@
       </c>
       <c r="O15" s="23">
         <f t="shared" si="0"/>
-        <v>0.89200000000000002</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="P15" s="8"/>
     </row>
@@ -12268,7 +12268,7 @@
       </c>
       <c r="O16" s="23">
         <f t="shared" si="0"/>
-        <v>0.91100000000000014</v>
+        <v>0.93300000000000016</v>
       </c>
       <c r="P16" s="8"/>
     </row>
@@ -12325,7 +12325,7 @@
       </c>
       <c r="O17" s="23">
         <f t="shared" si="0"/>
-        <v>0.87100000000000011</v>
+        <v>0.89300000000000013</v>
       </c>
       <c r="P17" s="8"/>
     </row>
@@ -12382,7 +12382,7 @@
       </c>
       <c r="O18" s="23">
         <f t="shared" si="0"/>
-        <v>0.91100000000000014</v>
+        <v>0.93300000000000016</v>
       </c>
       <c r="P18" s="8"/>
     </row>
@@ -12439,7 +12439,7 @@
       </c>
       <c r="O19" s="23">
         <f t="shared" si="0"/>
-        <v>0.84950000000000025</v>
+        <v>0.87150000000000027</v>
       </c>
       <c r="P19" s="8"/>
     </row>
@@ -12496,7 +12496,7 @@
       </c>
       <c r="O20" s="23">
         <f t="shared" si="0"/>
-        <v>0.90100000000000013</v>
+        <v>0.92300000000000015</v>
       </c>
       <c r="P20" s="8"/>
     </row>
@@ -12555,7 +12555,7 @@
       </c>
       <c r="O21" s="16">
         <f t="shared" si="0"/>
-        <v>0.85516666666666674</v>
+        <v>0.87711666666666666</v>
       </c>
       <c r="P21" s="14"/>
     </row>
@@ -12612,7 +12612,7 @@
       </c>
       <c r="O22" s="23">
         <f t="shared" si="0"/>
-        <v>0.77850000000000008</v>
+        <v>0.80045000000000011</v>
       </c>
       <c r="P22" s="8"/>
     </row>
@@ -12669,7 +12669,7 @@
       </c>
       <c r="O23" s="23">
         <f t="shared" si="0"/>
-        <v>0.82599999999999996</v>
+        <v>0.84795000000000009</v>
       </c>
       <c r="P23" s="8"/>
     </row>
@@ -12726,7 +12726,7 @@
       </c>
       <c r="O24" s="23">
         <f t="shared" si="0"/>
-        <v>0.8304999999999999</v>
+        <v>0.85245000000000004</v>
       </c>
       <c r="P24" s="8"/>
     </row>
@@ -12783,7 +12783,7 @@
       </c>
       <c r="O25" s="23">
         <f t="shared" si="0"/>
-        <v>0.84100000000000008</v>
+        <v>0.86294999999999999</v>
       </c>
       <c r="P25" s="8"/>
     </row>
@@ -12840,7 +12840,7 @@
       </c>
       <c r="O26" s="23">
         <f t="shared" si="0"/>
-        <v>0.85599999999999998</v>
+        <v>0.87795000000000012</v>
       </c>
       <c r="P26" s="8"/>
     </row>
@@ -12897,7 +12897,7 @@
       </c>
       <c r="O27" s="23">
         <f t="shared" si="0"/>
-        <v>0.87100000000000011</v>
+        <v>0.89295000000000002</v>
       </c>
       <c r="P27" s="8"/>
     </row>
@@ -12954,7 +12954,7 @@
       </c>
       <c r="O28" s="23">
         <f t="shared" si="0"/>
-        <v>0.86150000000000004</v>
+        <v>0.88345000000000018</v>
       </c>
       <c r="P28" s="8"/>
     </row>
@@ -13011,7 +13011,7 @@
       </c>
       <c r="O29" s="23">
         <f t="shared" si="0"/>
-        <v>0.87100000000000011</v>
+        <v>0.89295000000000002</v>
       </c>
       <c r="P29" s="8"/>
     </row>
@@ -13068,7 +13068,7 @@
       </c>
       <c r="O30" s="23">
         <f t="shared" si="0"/>
-        <v>0.86199999999999999</v>
+        <v>0.88395000000000012</v>
       </c>
       <c r="P30" s="8"/>
     </row>
@@ -13125,7 +13125,7 @@
       </c>
       <c r="O31" s="23">
         <f t="shared" si="0"/>
-        <v>0.87100000000000011</v>
+        <v>0.89295000000000002</v>
       </c>
       <c r="P31" s="8"/>
     </row>
@@ -13182,7 +13182,7 @@
       </c>
       <c r="O32" s="23">
         <f t="shared" si="0"/>
-        <v>0.85300000000000009</v>
+        <v>0.87495000000000001</v>
       </c>
       <c r="P32" s="8"/>
     </row>
@@ -13239,7 +13239,7 @@
       </c>
       <c r="O33" s="23">
         <f t="shared" si="0"/>
-        <v>0.87100000000000011</v>
+        <v>0.89295000000000002</v>
       </c>
       <c r="P33" s="8"/>
     </row>
@@ -13296,7 +13296,7 @@
       </c>
       <c r="O34" s="23">
         <f t="shared" si="0"/>
-        <v>0.84100000000000008</v>
+        <v>0.86295000000000011</v>
       </c>
       <c r="P34" s="8"/>
     </row>
@@ -13353,7 +13353,7 @@
       </c>
       <c r="O35" s="23">
         <f t="shared" ref="O35:O54" si="3">SUMPRODUCT(C35:N35, C$2:N$2)</f>
-        <v>0.87100000000000011</v>
+        <v>0.89295000000000002</v>
       </c>
       <c r="P35" s="8"/>
     </row>
@@ -13410,7 +13410,7 @@
       </c>
       <c r="O36" s="23">
         <f t="shared" si="3"/>
-        <v>0.83950000000000002</v>
+        <v>0.86145000000000016</v>
       </c>
       <c r="P36" s="8"/>
     </row>
@@ -13467,7 +13467,7 @@
       </c>
       <c r="O37" s="23">
         <f t="shared" si="3"/>
-        <v>0.86199999999999999</v>
+        <v>0.88395000000000012</v>
       </c>
       <c r="P37" s="8"/>
     </row>
@@ -13526,7 +13526,7 @@
       </c>
       <c r="O38" s="16">
         <f t="shared" si="3"/>
-        <v>0.81416666666666682</v>
+        <v>0.83598333333333352</v>
       </c>
       <c r="P38" s="14"/>
     </row>
@@ -13583,7 +13583,7 @@
       </c>
       <c r="O39" s="23">
         <f t="shared" si="3"/>
-        <v>0.71049999999999991</v>
+        <v>0.73245000000000005</v>
       </c>
       <c r="P39" s="8"/>
     </row>
@@ -13640,7 +13640,7 @@
       </c>
       <c r="O40" s="23">
         <f t="shared" si="3"/>
-        <v>0.8015000000000001</v>
+        <v>0.82345000000000002</v>
       </c>
       <c r="P40" s="8"/>
     </row>
@@ -13697,7 +13697,7 @@
       </c>
       <c r="O41" s="23">
         <f t="shared" si="3"/>
-        <v>0.82099999999999995</v>
+        <v>0.84295000000000009</v>
       </c>
       <c r="P41" s="8"/>
     </row>
@@ -13754,7 +13754,7 @@
       </c>
       <c r="O42" s="23">
         <f t="shared" si="3"/>
-        <v>0.76200000000000012</v>
+        <v>0.78195000000000014</v>
       </c>
       <c r="P42" s="8"/>
     </row>
@@ -13811,7 +13811,7 @@
       </c>
       <c r="O43" s="23">
         <f t="shared" si="3"/>
-        <v>0.8294999999999999</v>
+        <v>0.85145000000000004</v>
       </c>
       <c r="P43" s="8"/>
     </row>
@@ -13868,7 +13868,7 @@
       </c>
       <c r="O44" s="23">
         <f t="shared" si="3"/>
-        <v>0.80900000000000005</v>
+        <v>0.83094999999999997</v>
       </c>
       <c r="P44" s="8"/>
     </row>
@@ -13925,7 +13925,7 @@
       </c>
       <c r="O45" s="23">
         <f t="shared" si="3"/>
-        <v>0.83899999999999997</v>
+        <v>0.8609500000000001</v>
       </c>
       <c r="P45" s="8"/>
     </row>
@@ -13982,7 +13982,7 @@
       </c>
       <c r="O46" s="23">
         <f t="shared" si="3"/>
-        <v>0.84350000000000003</v>
+        <v>0.86545000000000016</v>
       </c>
       <c r="P46" s="8"/>
     </row>
@@ -14039,7 +14039,7 @@
       </c>
       <c r="O47" s="23">
         <f t="shared" si="3"/>
-        <v>0.82099999999999995</v>
+        <v>0.84295000000000009</v>
       </c>
       <c r="P47" s="8"/>
     </row>
@@ -14096,7 +14096,7 @@
       </c>
       <c r="O48" s="23">
         <f t="shared" si="3"/>
-        <v>0.84350000000000003</v>
+        <v>0.86545000000000016</v>
       </c>
       <c r="P48" s="8"/>
     </row>
@@ -14153,7 +14153,7 @@
       </c>
       <c r="O49" s="23">
         <f t="shared" si="3"/>
-        <v>0.82099999999999995</v>
+        <v>0.84295000000000009</v>
       </c>
       <c r="P49" s="8"/>
     </row>
@@ -14210,7 +14210,7 @@
       </c>
       <c r="O50" s="23">
         <f t="shared" si="3"/>
-        <v>0.85850000000000004</v>
+        <v>0.88045000000000018</v>
       </c>
       <c r="P50" s="8"/>
     </row>
@@ -14267,7 +14267,7 @@
       </c>
       <c r="O51" s="23">
         <f t="shared" si="3"/>
-        <v>0.72850000000000004</v>
+        <v>0.75044999999999995</v>
       </c>
       <c r="P51" s="8"/>
     </row>
@@ -14324,7 +14324,7 @@
       </c>
       <c r="O52" s="23">
         <f t="shared" si="3"/>
-        <v>0.82850000000000001</v>
+        <v>0.85045000000000015</v>
       </c>
       <c r="P52" s="8"/>
     </row>
@@ -14381,7 +14381,7 @@
       </c>
       <c r="O53" s="23">
         <f t="shared" si="3"/>
-        <v>0.78800000000000003</v>
+        <v>0.80995000000000017</v>
       </c>
       <c r="P53" s="8"/>
     </row>
@@ -14438,7 +14438,7 @@
       </c>
       <c r="O54" s="23">
         <f t="shared" si="3"/>
-        <v>0.81800000000000006</v>
+        <v>0.8399500000000002</v>
       </c>
       <c r="P54" s="8"/>
     </row>
@@ -14497,7 +14497,7 @@
       </c>
       <c r="O55" s="16">
         <f>AVERAGE(O56:O71)</f>
-        <v>0.78040624999999997</v>
+        <v>0.80235625000000022</v>
       </c>
       <c r="P55" s="14"/>
     </row>
@@ -14554,7 +14554,7 @@
       </c>
       <c r="O56" s="23">
         <f t="shared" ref="O56:O71" si="6">SUMPRODUCT(C56:N56, C$2:N$2)</f>
-        <v>0.79700000000000004</v>
+        <v>0.81895000000000007</v>
       </c>
       <c r="P56" s="8"/>
     </row>
@@ -14611,7 +14611,7 @@
       </c>
       <c r="O57" s="23">
         <f t="shared" si="6"/>
-        <v>0.76200000000000001</v>
+        <v>0.78395000000000004</v>
       </c>
       <c r="P57" s="8"/>
     </row>
@@ -14668,7 +14668,7 @@
       </c>
       <c r="O58" s="23">
         <f t="shared" si="6"/>
-        <v>0.78649999999999998</v>
+        <v>0.80845000000000011</v>
       </c>
       <c r="P58" s="8"/>
     </row>
@@ -14725,7 +14725,7 @@
       </c>
       <c r="O59" s="23">
         <f t="shared" si="6"/>
-        <v>0.75749999999999995</v>
+        <v>0.77945000000000009</v>
       </c>
       <c r="P59" s="8"/>
     </row>
@@ -14782,7 +14782,7 @@
       </c>
       <c r="O60" s="23">
         <f t="shared" si="6"/>
-        <v>0.77849999999999997</v>
+        <v>0.80045000000000011</v>
       </c>
       <c r="P60" s="8"/>
     </row>
@@ -14839,7 +14839,7 @@
       </c>
       <c r="O61" s="23">
         <f t="shared" si="6"/>
-        <v>0.75749999999999995</v>
+        <v>0.77945000000000009</v>
       </c>
       <c r="P61" s="8"/>
     </row>
@@ -14896,7 +14896,7 @@
       </c>
       <c r="O62" s="23">
         <f t="shared" si="6"/>
-        <v>0.79249999999999998</v>
+        <v>0.81445000000000001</v>
       </c>
       <c r="P62" s="8"/>
     </row>
@@ -14953,7 +14953,7 @@
       </c>
       <c r="O63" s="23">
         <f t="shared" si="6"/>
-        <v>0.79700000000000004</v>
+        <v>0.81895000000000007</v>
       </c>
       <c r="P63" s="8"/>
     </row>
@@ -15010,7 +15010,7 @@
       </c>
       <c r="O64" s="23">
         <f t="shared" si="6"/>
-        <v>0.79700000000000004</v>
+        <v>0.81895000000000007</v>
       </c>
       <c r="P64" s="8"/>
     </row>
@@ -15067,7 +15067,7 @@
       </c>
       <c r="O65" s="23">
         <f t="shared" si="6"/>
-        <v>0.78200000000000003</v>
+        <v>0.80395000000000005</v>
       </c>
       <c r="P65" s="8"/>
     </row>
@@ -15124,7 +15124,7 @@
       </c>
       <c r="O66" s="23">
         <f t="shared" si="6"/>
-        <v>0.77749999999999997</v>
+        <v>0.7994500000000001</v>
       </c>
       <c r="P66" s="8"/>
     </row>
@@ -15181,7 +15181,7 @@
       </c>
       <c r="O67" s="23">
         <f t="shared" si="6"/>
-        <v>0.79700000000000004</v>
+        <v>0.81895000000000007</v>
       </c>
       <c r="P67" s="8"/>
     </row>
@@ -15238,7 +15238,7 @@
       </c>
       <c r="O68" s="23">
         <f t="shared" si="6"/>
-        <v>0.79700000000000004</v>
+        <v>0.81895000000000007</v>
       </c>
       <c r="P68" s="8"/>
     </row>
@@ -15295,7 +15295,7 @@
       </c>
       <c r="O69" s="23">
         <f t="shared" si="6"/>
-        <v>0.77300000000000002</v>
+        <v>0.79495000000000005</v>
       </c>
       <c r="P69" s="8"/>
     </row>
@@ -15352,7 +15352,7 @@
       </c>
       <c r="O70" s="23">
         <f t="shared" si="6"/>
-        <v>0.748</v>
+        <v>0.76995000000000002</v>
       </c>
       <c r="P70" s="8"/>
     </row>
@@ -15409,7 +15409,7 @@
       </c>
       <c r="O71" s="23">
         <f t="shared" si="6"/>
-        <v>0.78649999999999998</v>
+        <v>0.80845000000000011</v>
       </c>
       <c r="P71" s="8"/>
     </row>
@@ -15468,7 +15468,7 @@
       </c>
       <c r="O72" s="16">
         <f>AVERAGE(O73:O88)</f>
-        <v>0.71778125000000015</v>
+        <v>0.73978125000000006</v>
       </c>
       <c r="P72" s="14"/>
     </row>
@@ -15525,7 +15525,7 @@
       </c>
       <c r="O73" s="23">
         <f t="shared" ref="O73:O88" si="8">SUMPRODUCT(C73:N73, C$2:N$2)</f>
-        <v>0.72500000000000009</v>
+        <v>0.74700000000000011</v>
       </c>
       <c r="P73" s="8"/>
     </row>
@@ -15582,7 +15582,7 @@
       </c>
       <c r="O74" s="23">
         <f t="shared" si="8"/>
-        <v>0.70300000000000018</v>
+        <v>0.7250000000000002</v>
       </c>
       <c r="P74" s="8"/>
     </row>
@@ -15639,7 +15639,7 @@
       </c>
       <c r="O75" s="23">
         <f t="shared" si="8"/>
-        <v>0.72550000000000014</v>
+        <v>0.74750000000000016</v>
       </c>
       <c r="P75" s="8"/>
     </row>
@@ -15696,7 +15696,7 @@
       </c>
       <c r="O76" s="23">
         <f t="shared" si="8"/>
-        <v>0.70450000000000002</v>
+        <v>0.72650000000000003</v>
       </c>
       <c r="P76" s="8"/>
     </row>
@@ -15753,7 +15753,7 @@
       </c>
       <c r="O77" s="23">
         <f t="shared" si="8"/>
-        <v>0.72550000000000014</v>
+        <v>0.74750000000000016</v>
       </c>
       <c r="P77" s="8"/>
     </row>
@@ -15810,7 +15810,7 @@
       </c>
       <c r="O78" s="23">
         <f t="shared" si="8"/>
-        <v>0.68750000000000011</v>
+        <v>0.70950000000000013</v>
       </c>
       <c r="P78" s="8"/>
     </row>
@@ -15867,7 +15867,7 @@
       </c>
       <c r="O79" s="23">
         <f t="shared" si="8"/>
-        <v>0.72550000000000014</v>
+        <v>0.74750000000000016</v>
       </c>
       <c r="P79" s="8"/>
     </row>
@@ -15924,7 +15924,7 @@
       </c>
       <c r="O80" s="23">
         <f t="shared" si="8"/>
-        <v>0.74500000000000011</v>
+        <v>0.76700000000000013</v>
       </c>
       <c r="P80" s="8"/>
     </row>
@@ -15981,7 +15981,7 @@
       </c>
       <c r="O81" s="23">
         <f t="shared" si="8"/>
-        <v>0.72400000000000009</v>
+        <v>0.74600000000000011</v>
       </c>
       <c r="P81" s="8"/>
     </row>
@@ -16038,7 +16038,7 @@
       </c>
       <c r="O82" s="23">
         <f t="shared" si="8"/>
-        <v>0.75400000000000011</v>
+        <v>0.77600000000000013</v>
       </c>
       <c r="P82" s="8"/>
     </row>
@@ -16095,7 +16095,7 @@
       </c>
       <c r="O83" s="23">
         <f t="shared" si="8"/>
-        <v>0.71850000000000014</v>
+        <v>0.74050000000000016</v>
       </c>
       <c r="P83" s="8"/>
     </row>
@@ -16152,7 +16152,7 @@
       </c>
       <c r="O84" s="23">
         <f t="shared" si="8"/>
-        <v>0.62050000000000005</v>
+        <v>0.64250000000000007</v>
       </c>
       <c r="P84" s="8"/>
     </row>
@@ -16209,7 +16209,7 @@
       </c>
       <c r="O85" s="23">
         <f t="shared" si="8"/>
-        <v>0.72550000000000014</v>
+        <v>0.74750000000000016</v>
       </c>
       <c r="P85" s="8"/>
     </row>
@@ -16266,7 +16266,7 @@
       </c>
       <c r="O86" s="23">
         <f t="shared" si="8"/>
-        <v>0.74350000000000016</v>
+        <v>0.76550000000000018</v>
       </c>
       <c r="P86" s="8"/>
     </row>
@@ -16323,7 +16323,7 @@
       </c>
       <c r="O87" s="23">
         <f t="shared" si="8"/>
-        <v>0.70300000000000018</v>
+        <v>0.7250000000000002</v>
       </c>
       <c r="P87" s="8"/>
     </row>
@@ -16380,7 +16380,7 @@
       </c>
       <c r="O88" s="23">
         <f t="shared" si="8"/>
-        <v>0.75400000000000011</v>
+        <v>0.77600000000000013</v>
       </c>
       <c r="P88" s="8"/>
     </row>
@@ -16439,7 +16439,7 @@
       </c>
       <c r="O89" s="16">
         <f>AVERAGE(O90:O105)</f>
-        <v>0.71421875000000001</v>
+        <v>0.73620625000000006</v>
       </c>
       <c r="P89" s="14"/>
     </row>
@@ -16496,7 +16496,7 @@
       </c>
       <c r="O90" s="23">
         <f t="shared" ref="O90:O105" si="10">SUMPRODUCT(C90:N90, C$2:N$2)</f>
-        <v>0.68300000000000016</v>
+        <v>0.70500000000000018</v>
       </c>
       <c r="P90" s="8"/>
     </row>
@@ -16553,7 +16553,7 @@
       </c>
       <c r="O91" s="23">
         <f t="shared" si="10"/>
-        <v>0.72400000000000009</v>
+        <v>0.74600000000000011</v>
       </c>
       <c r="P91" s="8"/>
     </row>
@@ -16610,7 +16610,7 @@
       </c>
       <c r="O92" s="23">
         <f t="shared" si="10"/>
-        <v>0.63550000000000018</v>
+        <v>0.65749999999999997</v>
       </c>
       <c r="P92" s="8"/>
     </row>
@@ -16667,7 +16667,7 @@
       </c>
       <c r="O93" s="23">
         <f t="shared" si="10"/>
-        <v>0.70900000000000007</v>
+        <v>0.73100000000000009</v>
       </c>
       <c r="P93" s="8"/>
     </row>
@@ -16724,7 +16724,7 @@
       </c>
       <c r="O94" s="23">
         <f t="shared" si="10"/>
-        <v>0.72550000000000014</v>
+        <v>0.74750000000000016</v>
       </c>
       <c r="P94" s="8"/>
     </row>
@@ -16781,7 +16781,7 @@
       </c>
       <c r="O95" s="23">
         <f t="shared" si="10"/>
-        <v>0.70900000000000007</v>
+        <v>0.73100000000000009</v>
       </c>
       <c r="P95" s="8"/>
     </row>
@@ -16838,7 +16838,7 @@
       </c>
       <c r="O96" s="23">
         <f t="shared" si="10"/>
-        <v>0.72550000000000014</v>
+        <v>0.74750000000000016</v>
       </c>
       <c r="P96" s="8"/>
     </row>
@@ -16895,7 +16895,7 @@
       </c>
       <c r="O97" s="23">
         <f t="shared" si="10"/>
-        <v>0.70900000000000007</v>
+        <v>0.73100000000000009</v>
       </c>
       <c r="P97" s="8"/>
     </row>
@@ -16952,7 +16952,7 @@
       </c>
       <c r="O98" s="23">
         <f t="shared" si="10"/>
-        <v>0.72550000000000014</v>
+        <v>0.74750000000000016</v>
       </c>
       <c r="P98" s="8"/>
     </row>
@@ -17009,7 +17009,7 @@
       </c>
       <c r="O99" s="23">
         <f t="shared" si="10"/>
-        <v>0.75400000000000011</v>
+        <v>0.77600000000000013</v>
       </c>
       <c r="P99" s="8"/>
     </row>
@@ -17066,7 +17066,7 @@
       </c>
       <c r="O100" s="23">
         <f t="shared" si="10"/>
-        <v>0.72450000000000003</v>
+        <v>0.74640000000000006</v>
       </c>
       <c r="P100" s="8"/>
     </row>
@@ -17123,7 +17123,7 @@
       </c>
       <c r="O101" s="23">
         <f t="shared" si="10"/>
-        <v>0.75400000000000011</v>
+        <v>0.77600000000000013</v>
       </c>
       <c r="P101" s="8"/>
     </row>
@@ -17180,7 +17180,7 @@
       </c>
       <c r="O102" s="23">
         <f t="shared" si="10"/>
-        <v>0.70450000000000013</v>
+        <v>0.72650000000000015</v>
       </c>
       <c r="P102" s="8"/>
     </row>
@@ -17237,7 +17237,7 @@
       </c>
       <c r="O103" s="23">
         <f t="shared" si="10"/>
-        <v>0.75400000000000011</v>
+        <v>0.77600000000000013</v>
       </c>
       <c r="P103" s="8"/>
     </row>
@@ -17294,7 +17294,7 @@
       </c>
       <c r="O104" s="23">
         <f t="shared" si="10"/>
-        <v>0.70300000000000018</v>
+        <v>0.7250000000000002</v>
       </c>
       <c r="P104" s="8"/>
     </row>
@@ -17351,7 +17351,7 @@
       </c>
       <c r="O105" s="23">
         <f t="shared" si="10"/>
-        <v>0.68750000000000011</v>
+        <v>0.70940000000000003</v>
       </c>
       <c r="P105" s="8"/>
     </row>
@@ -17410,7 +17410,7 @@
       </c>
       <c r="O106" s="16">
         <f>AVERAGE(O107:O122)</f>
-        <v>0.60476562500000008</v>
+        <v>0.6265281250000001</v>
       </c>
       <c r="P106" s="14"/>
     </row>
@@ -17467,7 +17467,7 @@
       </c>
       <c r="O107" s="23">
         <f t="shared" ref="O107:O122" si="12">SUMPRODUCT(C107:N107, C$2:N$2)</f>
-        <v>0.56625000000000003</v>
+        <v>0.58820000000000006</v>
       </c>
       <c r="P107" s="8"/>
     </row>
@@ -17524,7 +17524,7 @@
       </c>
       <c r="O108" s="23">
         <f t="shared" si="12"/>
-        <v>0.58950000000000014</v>
+        <v>0.61145000000000005</v>
       </c>
       <c r="P108" s="8"/>
     </row>
@@ -17581,7 +17581,7 @@
       </c>
       <c r="O109" s="23">
         <f t="shared" si="12"/>
-        <v>0.60850000000000004</v>
+        <v>0.63044999999999995</v>
       </c>
       <c r="P109" s="8"/>
     </row>
@@ -17638,7 +17638,7 @@
       </c>
       <c r="O110" s="23">
         <f t="shared" si="12"/>
-        <v>0.56750000000000012</v>
+        <v>0.58845000000000014</v>
       </c>
       <c r="P110" s="8"/>
     </row>
@@ -17695,7 +17695,7 @@
       </c>
       <c r="O111" s="23">
         <f t="shared" si="12"/>
-        <v>0.60350000000000004</v>
+        <v>0.62545000000000006</v>
       </c>
       <c r="P111" s="8"/>
     </row>
@@ -17752,7 +17752,7 @@
       </c>
       <c r="O112" s="23">
         <f t="shared" si="12"/>
-        <v>0.59250000000000003</v>
+        <v>0.61245000000000016</v>
       </c>
       <c r="P112" s="8"/>
     </row>
@@ -17809,7 +17809,7 @@
       </c>
       <c r="O113" s="23">
         <f t="shared" si="12"/>
-        <v>0.62450000000000006</v>
+        <v>0.64644999999999997</v>
       </c>
       <c r="P113" s="8"/>
     </row>
@@ -17866,7 +17866,7 @@
       </c>
       <c r="O114" s="23">
         <f t="shared" si="12"/>
-        <v>0.65000000000000013</v>
+        <v>0.67195000000000005</v>
       </c>
       <c r="P114" s="8"/>
     </row>
@@ -17923,7 +17923,7 @@
       </c>
       <c r="O115" s="23">
         <f t="shared" si="12"/>
-        <v>0.625</v>
+        <v>0.64695000000000014</v>
       </c>
       <c r="P115" s="8"/>
     </row>
@@ -17980,7 +17980,7 @@
       </c>
       <c r="O116" s="23">
         <f t="shared" si="12"/>
-        <v>0.65300000000000002</v>
+        <v>0.67495000000000016</v>
       </c>
       <c r="P116" s="8"/>
     </row>
@@ -18037,7 +18037,7 @@
       </c>
       <c r="O117" s="23">
         <f t="shared" si="12"/>
-        <v>0.58250000000000002</v>
+        <v>0.60445000000000015</v>
       </c>
       <c r="P117" s="8"/>
     </row>
@@ -18094,7 +18094,7 @@
       </c>
       <c r="O118" s="23">
         <f t="shared" si="12"/>
-        <v>0.64250000000000007</v>
+        <v>0.66444999999999999</v>
       </c>
       <c r="P118" s="8"/>
     </row>
@@ -18151,7 +18151,7 @@
       </c>
       <c r="O119" s="23">
         <f t="shared" si="12"/>
-        <v>0.55700000000000005</v>
+        <v>0.57895000000000008</v>
       </c>
       <c r="P119" s="8"/>
     </row>
@@ -18208,7 +18208,7 @@
       </c>
       <c r="O120" s="23">
         <f t="shared" si="12"/>
-        <v>0.65250000000000008</v>
+        <v>0.67444999999999999</v>
       </c>
       <c r="P120" s="8"/>
     </row>
@@ -18265,7 +18265,7 @@
       </c>
       <c r="O121" s="23">
         <f t="shared" si="12"/>
-        <v>0.55700000000000005</v>
+        <v>0.57895000000000008</v>
       </c>
       <c r="P121" s="8"/>
     </row>
@@ -18322,7 +18322,7 @@
       </c>
       <c r="O122" s="23">
         <f t="shared" si="12"/>
-        <v>0.60450000000000004</v>
+        <v>0.62645000000000017</v>
       </c>
       <c r="P122" s="8"/>
     </row>
@@ -18381,7 +18381,7 @@
       </c>
       <c r="O123" s="15">
         <f>AVERAGE(O124:O139)</f>
-        <v>0.5424062500000002</v>
+        <v>0.56435625</v>
       </c>
       <c r="P123" s="14"/>
     </row>
@@ -18438,7 +18438,7 @@
       </c>
       <c r="O124" s="23">
         <f t="shared" ref="O124:O139" si="14">SUMPRODUCT(C124:N124, C$2:N$2)</f>
-        <v>0.58250000000000002</v>
+        <v>0.60445000000000015</v>
       </c>
       <c r="P124" s="8"/>
     </row>
@@ -18495,7 +18495,7 @@
       </c>
       <c r="O125" s="23">
         <f t="shared" si="14"/>
-        <v>0.58000000000000007</v>
+        <v>0.60194999999999999</v>
       </c>
       <c r="P125" s="8"/>
     </row>
@@ -18552,7 +18552,7 @@
       </c>
       <c r="O126" s="23">
         <f t="shared" si="14"/>
-        <v>0.58250000000000002</v>
+        <v>0.60445000000000015</v>
       </c>
       <c r="P126" s="8"/>
     </row>
@@ -18609,7 +18609,7 @@
       </c>
       <c r="O127" s="23">
         <f t="shared" si="14"/>
-        <v>0.45250000000000001</v>
+        <v>0.47445000000000004</v>
       </c>
       <c r="P127" s="8"/>
     </row>
@@ -18666,7 +18666,7 @@
       </c>
       <c r="O128" s="23">
         <f t="shared" si="14"/>
-        <v>0.56750000000000012</v>
+        <v>0.58945000000000003</v>
       </c>
       <c r="P128" s="8"/>
     </row>
@@ -18723,7 +18723,7 @@
       </c>
       <c r="O129" s="23">
         <f t="shared" si="14"/>
-        <v>0.56800000000000006</v>
+        <v>0.58994999999999997</v>
       </c>
       <c r="P129" s="8"/>
     </row>
@@ -18780,7 +18780,7 @@
       </c>
       <c r="O130" s="23">
         <f t="shared" si="14"/>
-        <v>0.55800000000000005</v>
+        <v>0.57995000000000008</v>
       </c>
       <c r="P130" s="8"/>
     </row>
@@ -18837,7 +18837,7 @@
       </c>
       <c r="O131" s="23">
         <f t="shared" si="14"/>
-        <v>0.58250000000000002</v>
+        <v>0.60445000000000015</v>
       </c>
       <c r="P131" s="8"/>
     </row>
@@ -18894,7 +18894,7 @@
       </c>
       <c r="O132" s="23">
         <f t="shared" si="14"/>
-        <v>0.64250000000000007</v>
+        <v>0.66444999999999999</v>
       </c>
       <c r="P132" s="8"/>
     </row>
@@ -18951,7 +18951,7 @@
       </c>
       <c r="O133" s="23">
         <f t="shared" si="14"/>
-        <v>0.59750000000000014</v>
+        <v>0.61945000000000006</v>
       </c>
       <c r="P133" s="8"/>
     </row>
@@ -19008,7 +19008,7 @@
       </c>
       <c r="O134" s="23">
         <f t="shared" si="14"/>
-        <v>0.51050000000000006</v>
+        <v>0.53245000000000009</v>
       </c>
       <c r="P134" s="8"/>
     </row>
@@ -19065,7 +19065,7 @@
       </c>
       <c r="O135" s="23">
         <f t="shared" si="14"/>
-        <v>0.64250000000000007</v>
+        <v>0.66444999999999999</v>
       </c>
       <c r="P135" s="8"/>
     </row>
@@ -19122,7 +19122,7 @@
       </c>
       <c r="O136" s="23">
         <f t="shared" si="14"/>
-        <v>0.43250000000000005</v>
+        <v>0.45445000000000008</v>
       </c>
       <c r="P136" s="8"/>
     </row>
@@ -19179,7 +19179,7 @@
       </c>
       <c r="O137" s="23">
         <f t="shared" si="14"/>
-        <v>0.503</v>
+        <v>0.52495000000000003</v>
       </c>
       <c r="P137" s="8"/>
     </row>
@@ -19236,7 +19236,7 @@
       </c>
       <c r="O138" s="23">
         <f t="shared" si="14"/>
-        <v>0.40350000000000003</v>
+        <v>0.42545000000000005</v>
       </c>
       <c r="P138" s="8"/>
     </row>
@@ -19293,7 +19293,7 @@
       </c>
       <c r="O139" s="23">
         <f t="shared" si="14"/>
-        <v>0.47300000000000003</v>
+        <v>0.49495000000000006</v>
       </c>
       <c r="P139" s="8"/>
     </row>
@@ -19352,7 +19352,7 @@
       </c>
       <c r="O140" s="16">
         <f>AVERAGE(O141:O156)</f>
-        <v>0.40712500000000001</v>
+        <v>0.42604062500000006</v>
       </c>
       <c r="P140" s="14"/>
     </row>
@@ -19409,7 +19409,7 @@
       </c>
       <c r="O141" s="23">
         <f t="shared" ref="O141:O156" si="16">SUMPRODUCT(C141:N141, C$2:N$2)</f>
-        <v>0.4830000000000001</v>
+        <v>0.50195000000000001</v>
       </c>
       <c r="P141" s="8"/>
     </row>
@@ -19466,7 +19466,7 @@
       </c>
       <c r="O142" s="23">
         <f t="shared" si="16"/>
-        <v>0.38450000000000006</v>
+        <v>0.40245000000000003</v>
       </c>
       <c r="P142" s="8"/>
     </row>
@@ -19523,7 +19523,7 @@
       </c>
       <c r="O143" s="23">
         <f t="shared" si="16"/>
-        <v>0.49750000000000011</v>
+        <v>0.51544999999999996</v>
       </c>
       <c r="P143" s="8"/>
     </row>
@@ -19580,7 +19580,7 @@
       </c>
       <c r="O144" s="23">
         <f t="shared" si="16"/>
-        <v>0.4195000000000001</v>
+        <v>0.43745000000000001</v>
       </c>
       <c r="P144" s="8"/>
     </row>
@@ -19637,7 +19637,7 @@
       </c>
       <c r="O145" s="23">
         <f t="shared" si="16"/>
-        <v>0.40800000000000003</v>
+        <v>0.42995000000000005</v>
       </c>
       <c r="P145" s="8"/>
     </row>
@@ -19694,7 +19694,7 @@
       </c>
       <c r="O146" s="23">
         <f t="shared" si="16"/>
-        <v>0.43200000000000005</v>
+        <v>0.44995000000000002</v>
       </c>
       <c r="P146" s="8"/>
     </row>
@@ -19751,7 +19751,7 @@
       </c>
       <c r="O147" s="23">
         <f t="shared" si="16"/>
-        <v>0.39250000000000002</v>
+        <v>0.41045000000000004</v>
       </c>
       <c r="P147" s="8"/>
     </row>
@@ -19808,7 +19808,7 @@
       </c>
       <c r="O148" s="23">
         <f t="shared" si="16"/>
-        <v>0.5665</v>
+        <v>0.58845000000000014</v>
       </c>
       <c r="P148" s="8"/>
     </row>
@@ -19865,7 +19865,7 @@
       </c>
       <c r="O149" s="23">
         <f t="shared" si="16"/>
-        <v>0.36800000000000005</v>
+        <v>0.38595000000000002</v>
       </c>
       <c r="P149" s="8"/>
     </row>
@@ -19922,7 +19922,7 @@
       </c>
       <c r="O150" s="23">
         <f t="shared" si="16"/>
-        <v>0.42800000000000005</v>
+        <v>0.44595000000000001</v>
       </c>
       <c r="P150" s="8"/>
     </row>
@@ -19979,7 +19979,7 @@
       </c>
       <c r="O151" s="23">
         <f t="shared" si="16"/>
-        <v>0.37250000000000005</v>
+        <v>0.39445000000000008</v>
       </c>
       <c r="P151" s="8"/>
     </row>
@@ -20036,7 +20036,7 @@
       </c>
       <c r="O152" s="23">
         <f t="shared" si="16"/>
-        <v>0.33250000000000002</v>
+        <v>0.35045000000000004</v>
       </c>
       <c r="P152" s="8"/>
     </row>
@@ -20093,7 +20093,7 @@
       </c>
       <c r="O153" s="23">
         <f t="shared" si="16"/>
-        <v>0.34800000000000003</v>
+        <v>0.36995000000000006</v>
       </c>
       <c r="P153" s="8"/>
     </row>
@@ -20150,7 +20150,7 @@
       </c>
       <c r="O154" s="23">
         <f t="shared" si="16"/>
-        <v>0.39250000000000007</v>
+        <v>0.41044999999999998</v>
       </c>
       <c r="P154" s="8"/>
     </row>
@@ -20207,7 +20207,7 @@
       </c>
       <c r="O155" s="23">
         <f t="shared" si="16"/>
-        <v>0.27450000000000002</v>
+        <v>0.28689999999999999</v>
       </c>
       <c r="P155" s="8"/>
     </row>
@@ -20264,7 +20264,7 @@
       </c>
       <c r="O156" s="23">
         <f t="shared" si="16"/>
-        <v>0.41450000000000004</v>
+        <v>0.43645000000000006</v>
       </c>
       <c r="P156" s="8"/>
     </row>
@@ -20323,7 +20323,7 @@
       </c>
       <c r="O157" s="15">
         <f>AVERAGE(O158:O173)</f>
-        <v>0.21106249999999999</v>
+        <v>0.21944374999999999</v>
       </c>
       <c r="P157" s="14"/>
     </row>
@@ -20380,7 +20380,7 @@
       </c>
       <c r="O158" s="23">
         <f t="shared" ref="O158:O173" si="18">SUMPRODUCT(C158:N158, C$2:N$2)</f>
-        <v>0.17850000000000002</v>
+        <v>0.18350000000000002</v>
       </c>
       <c r="P158" s="8"/>
     </row>
@@ -20437,7 +20437,7 @@
       </c>
       <c r="O159" s="23">
         <f t="shared" si="18"/>
-        <v>0.22700000000000001</v>
+        <v>0.23694999999999999</v>
       </c>
       <c r="P159" s="8"/>
     </row>
@@ -20494,7 +20494,7 @@
       </c>
       <c r="O160" s="23">
         <f t="shared" si="18"/>
-        <v>0.14850000000000002</v>
+        <v>0.15050000000000002</v>
       </c>
       <c r="P160" s="8"/>
     </row>
@@ -20551,7 +20551,7 @@
       </c>
       <c r="O161" s="23">
         <f t="shared" si="18"/>
-        <v>0.21249999999999999</v>
+        <v>0.22100000000000003</v>
       </c>
       <c r="P161" s="8"/>
     </row>
@@ -20608,7 +20608,7 @@
       </c>
       <c r="O162" s="23">
         <f t="shared" si="18"/>
-        <v>0.2135</v>
+        <v>0.22200000000000003</v>
       </c>
       <c r="P162" s="8"/>
     </row>
@@ -20665,7 +20665,7 @@
       </c>
       <c r="O163" s="23">
         <f t="shared" si="18"/>
-        <v>0.22700000000000001</v>
+        <v>0.23694999999999999</v>
       </c>
       <c r="P163" s="8"/>
     </row>
@@ -20722,7 +20722,7 @@
       </c>
       <c r="O164" s="23">
         <f t="shared" si="18"/>
-        <v>0.2135</v>
+        <v>0.22200000000000003</v>
       </c>
       <c r="P164" s="8"/>
     </row>
@@ -20779,7 +20779,7 @@
       </c>
       <c r="O165" s="23">
         <f t="shared" si="18"/>
-        <v>0.22700000000000001</v>
+        <v>0.23694999999999999</v>
       </c>
       <c r="P165" s="8"/>
     </row>
@@ -20836,7 +20836,7 @@
       </c>
       <c r="O166" s="23">
         <f t="shared" si="18"/>
-        <v>0.22800000000000001</v>
+        <v>0.23794999999999999</v>
       </c>
       <c r="P166" s="8"/>
     </row>
@@ -20893,7 +20893,7 @@
       </c>
       <c r="O167" s="23">
         <f t="shared" si="18"/>
-        <v>0.2135</v>
+        <v>0.22200000000000003</v>
       </c>
       <c r="P167" s="8"/>
     </row>
@@ -20950,7 +20950,7 @@
       </c>
       <c r="O168" s="23">
         <f t="shared" si="18"/>
-        <v>0.2135</v>
+        <v>0.22200000000000003</v>
       </c>
       <c r="P168" s="8"/>
     </row>
@@ -21007,7 +21007,7 @@
       </c>
       <c r="O169" s="23">
         <f t="shared" si="18"/>
-        <v>0.2235</v>
+        <v>0.23344999999999999</v>
       </c>
       <c r="P169" s="8"/>
     </row>
@@ -21064,7 +21064,7 @@
       </c>
       <c r="O170" s="23">
         <f t="shared" si="18"/>
-        <v>0.25800000000000001</v>
+        <v>0.27095000000000002</v>
       </c>
       <c r="P170" s="8"/>
     </row>
@@ -21121,7 +21121,7 @@
       </c>
       <c r="O171" s="23">
         <f t="shared" si="18"/>
-        <v>0.2235</v>
+        <v>0.23344999999999999</v>
       </c>
       <c r="P171" s="8"/>
     </row>
@@ -21178,7 +21178,7 @@
       </c>
       <c r="O172" s="23">
         <f t="shared" si="18"/>
-        <v>0.14600000000000002</v>
+        <v>0.14800000000000002</v>
       </c>
       <c r="P172" s="8"/>
     </row>
@@ -21235,7 +21235,7 @@
       </c>
       <c r="O173" s="23">
         <f t="shared" si="18"/>
-        <v>0.2235</v>
+        <v>0.23344999999999999</v>
       </c>
       <c r="P173" s="8"/>
     </row>
@@ -21343,7 +21343,7 @@
       </c>
       <c r="O175" s="23">
         <f t="shared" ref="O175:O190" si="20">SUMPRODUCT(C175:N175, C$2:N$2)</f>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P175" s="8"/>
     </row>
@@ -21392,7 +21392,7 @@
       </c>
       <c r="O176" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P176" s="8"/>
     </row>
@@ -21441,7 +21441,7 @@
       </c>
       <c r="O177" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P177" s="8"/>
     </row>
@@ -21490,7 +21490,7 @@
       </c>
       <c r="O178" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P178" s="8"/>
     </row>
@@ -21539,7 +21539,7 @@
       </c>
       <c r="O179" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P179" s="8"/>
     </row>
@@ -21588,7 +21588,7 @@
       </c>
       <c r="O180" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P180" s="8"/>
     </row>
@@ -21637,7 +21637,7 @@
       </c>
       <c r="O181" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P181" s="8"/>
     </row>
@@ -21686,7 +21686,7 @@
       </c>
       <c r="O182" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P182" s="8"/>
     </row>
@@ -21735,7 +21735,7 @@
       </c>
       <c r="O183" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P183" s="8"/>
     </row>
@@ -21784,7 +21784,7 @@
       </c>
       <c r="O184" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P184" s="8"/>
     </row>
@@ -21833,7 +21833,7 @@
       </c>
       <c r="O185" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P185" s="8"/>
     </row>
@@ -21882,7 +21882,7 @@
       </c>
       <c r="O186" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P186" s="8"/>
     </row>
@@ -21931,7 +21931,7 @@
       </c>
       <c r="O187" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P187" s="8"/>
     </row>
@@ -21980,7 +21980,7 @@
       </c>
       <c r="O188" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P188" s="8"/>
     </row>
@@ -22029,7 +22029,7 @@
       </c>
       <c r="O189" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P189" s="8"/>
     </row>
@@ -22078,7 +22078,7 @@
       </c>
       <c r="O190" s="23">
         <f t="shared" si="20"/>
-        <v>0.13400000000000001</v>
+        <v>0.13399999999999998</v>
       </c>
       <c r="P190" s="9"/>
     </row>
@@ -22141,11 +22141,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A174:B174"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="A3:B3"/>
@@ -22153,6 +22148,11 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A174:B174"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="19" orientation="landscape" r:id="rId1"/>
@@ -22205,81 +22205,81 @@
       </c>
     </row>
     <row r="2" spans="2:59" ht="24.75" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="203" t="s">
+      <c r="C2" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="204"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="206"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="181"/>
       <c r="G2" s="36"/>
-      <c r="H2" s="207" t="s">
+      <c r="H2" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="204"/>
-      <c r="J2" s="205"/>
-      <c r="K2" s="205"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
       <c r="L2" s="36"/>
-      <c r="M2" s="203" t="s">
+      <c r="M2" s="178" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="204"/>
-      <c r="O2" s="205"/>
-      <c r="P2" s="206"/>
-      <c r="Q2" s="203" t="s">
+      <c r="N2" s="179"/>
+      <c r="O2" s="180"/>
+      <c r="P2" s="181"/>
+      <c r="Q2" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="204"/>
-      <c r="S2" s="205"/>
-      <c r="T2" s="206"/>
-      <c r="U2" s="203" t="s">
+      <c r="R2" s="179"/>
+      <c r="S2" s="180"/>
+      <c r="T2" s="181"/>
+      <c r="U2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="204"/>
-      <c r="W2" s="205"/>
-      <c r="X2" s="206"/>
+      <c r="V2" s="179"/>
+      <c r="W2" s="180"/>
+      <c r="X2" s="181"/>
       <c r="Y2" s="36"/>
-      <c r="Z2" s="178" t="s">
+      <c r="Z2" s="183" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="179"/>
-      <c r="AB2" s="179"/>
-      <c r="AC2" s="180"/>
+      <c r="AA2" s="184"/>
+      <c r="AB2" s="184"/>
+      <c r="AC2" s="185"/>
       <c r="AD2" s="36"/>
-      <c r="AE2" s="179" t="s">
+      <c r="AE2" s="184" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="179"/>
-      <c r="AH2" s="179"/>
+      <c r="AF2" s="184"/>
+      <c r="AG2" s="184"/>
+      <c r="AH2" s="184"/>
       <c r="AI2" s="36"/>
-      <c r="AJ2" s="208" t="s">
+      <c r="AJ2" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="AK2" s="209"/>
-      <c r="AL2" s="209"/>
-      <c r="AM2" s="178" t="s">
+      <c r="AK2" s="187"/>
+      <c r="AL2" s="187"/>
+      <c r="AM2" s="183" t="s">
         <v>55</v>
       </c>
-      <c r="AN2" s="179"/>
-      <c r="AO2" s="179"/>
-      <c r="AP2" s="180"/>
+      <c r="AN2" s="184"/>
+      <c r="AO2" s="184"/>
+      <c r="AP2" s="185"/>
       <c r="AQ2" s="36"/>
-      <c r="AR2" s="178" t="s">
+      <c r="AR2" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AS2" s="179"/>
-      <c r="AT2" s="179"/>
-      <c r="AU2" s="180"/>
+      <c r="AS2" s="184"/>
+      <c r="AT2" s="184"/>
+      <c r="AU2" s="185"/>
       <c r="AV2" s="36"/>
-      <c r="AW2" s="181" t="s">
+      <c r="AW2" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="AX2" s="182"/>
-      <c r="AY2" s="183"/>
+      <c r="AX2" s="176"/>
+      <c r="AY2" s="177"/>
       <c r="AZ2" s="37"/>
-      <c r="BA2" s="181"/>
-      <c r="BB2" s="182"/>
-      <c r="BC2" s="183"/>
+      <c r="BA2" s="175"/>
+      <c r="BB2" s="176"/>
+      <c r="BC2" s="177"/>
       <c r="BD2" s="38"/>
     </row>
     <row r="3" spans="2:59" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -22487,10 +22487,10 @@
       <c r="R8" s="59"/>
       <c r="S8" s="59"/>
       <c r="T8" s="59"/>
-      <c r="U8" s="211"/>
-      <c r="V8" s="211"/>
-      <c r="W8" s="211"/>
-      <c r="X8" s="211"/>
+      <c r="U8" s="173"/>
+      <c r="V8" s="173"/>
+      <c r="W8" s="173"/>
+      <c r="X8" s="173"/>
       <c r="Y8" s="60"/>
       <c r="Z8" s="60"/>
       <c r="AA8" s="60"/>
@@ -22505,13 +22505,13 @@
       <c r="AJ8" s="60"/>
       <c r="AK8" s="60"/>
       <c r="AL8" s="60"/>
-      <c r="AM8" s="212">
+      <c r="AM8" s="174">
         <f ca="1">NOW()</f>
-        <v>45995.961089236109</v>
-      </c>
-      <c r="AN8" s="211"/>
-      <c r="AO8" s="211"/>
-      <c r="AP8" s="211"/>
+        <v>45995.967272337963</v>
+      </c>
+      <c r="AN8" s="173"/>
+      <c r="AO8" s="173"/>
+      <c r="AP8" s="173"/>
       <c r="AQ8" s="61"/>
       <c r="AR8" s="61"/>
       <c r="AS8" s="61"/>
@@ -22522,139 +22522,139 @@
       <c r="AX8" s="61"/>
       <c r="AY8" s="61"/>
       <c r="AZ8" s="61"/>
-      <c r="BA8" s="211"/>
-      <c r="BB8" s="211"/>
+      <c r="BA8" s="173"/>
+      <c r="BB8" s="173"/>
       <c r="BC8" s="62"/>
       <c r="BD8" s="62"/>
-      <c r="BE8" s="191"/>
-      <c r="BF8" s="191"/>
+      <c r="BE8" s="188"/>
+      <c r="BF8" s="188"/>
       <c r="BG8" s="63" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="192" t="s">
+      <c r="B9" s="189" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="193"/>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="193"/>
-      <c r="I9" s="193"/>
-      <c r="J9" s="193"/>
-      <c r="K9" s="193"/>
-      <c r="L9" s="193"/>
-      <c r="M9" s="194"/>
-      <c r="N9" s="194"/>
-      <c r="O9" s="194"/>
-      <c r="P9" s="194"/>
-      <c r="Q9" s="195"/>
-      <c r="R9" s="195"/>
-      <c r="S9" s="195"/>
-      <c r="T9" s="195"/>
-      <c r="U9" s="195"/>
-      <c r="V9" s="195"/>
-      <c r="W9" s="195"/>
-      <c r="X9" s="195"/>
-      <c r="Y9" s="195"/>
-      <c r="Z9" s="195"/>
-      <c r="AA9" s="195"/>
-      <c r="AB9" s="195"/>
-      <c r="AC9" s="195"/>
-      <c r="AD9" s="195"/>
-      <c r="AE9" s="195"/>
-      <c r="AF9" s="195"/>
-      <c r="AG9" s="195"/>
-      <c r="AH9" s="195"/>
-      <c r="AI9" s="195"/>
-      <c r="AJ9" s="195"/>
-      <c r="AK9" s="195"/>
-      <c r="AL9" s="195"/>
-      <c r="AM9" s="195"/>
-      <c r="AN9" s="195"/>
-      <c r="AO9" s="195"/>
-      <c r="AP9" s="195"/>
-      <c r="AQ9" s="195"/>
-      <c r="AR9" s="195"/>
-      <c r="AS9" s="195"/>
-      <c r="AT9" s="195"/>
-      <c r="AU9" s="195"/>
-      <c r="AV9" s="195"/>
-      <c r="AW9" s="195"/>
-      <c r="AX9" s="195"/>
-      <c r="AY9" s="195"/>
-      <c r="AZ9" s="195"/>
-      <c r="BA9" s="195"/>
-      <c r="BB9" s="195"/>
-      <c r="BC9" s="195"/>
-      <c r="BD9" s="195"/>
-      <c r="BE9" s="195"/>
-      <c r="BF9" s="195"/>
-      <c r="BG9" s="196"/>
+      <c r="C9" s="190"/>
+      <c r="D9" s="190"/>
+      <c r="E9" s="190"/>
+      <c r="F9" s="190"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="190"/>
+      <c r="I9" s="190"/>
+      <c r="J9" s="190"/>
+      <c r="K9" s="190"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="191"/>
+      <c r="N9" s="191"/>
+      <c r="O9" s="191"/>
+      <c r="P9" s="191"/>
+      <c r="Q9" s="192"/>
+      <c r="R9" s="192"/>
+      <c r="S9" s="192"/>
+      <c r="T9" s="192"/>
+      <c r="U9" s="192"/>
+      <c r="V9" s="192"/>
+      <c r="W9" s="192"/>
+      <c r="X9" s="192"/>
+      <c r="Y9" s="192"/>
+      <c r="Z9" s="192"/>
+      <c r="AA9" s="192"/>
+      <c r="AB9" s="192"/>
+      <c r="AC9" s="192"/>
+      <c r="AD9" s="192"/>
+      <c r="AE9" s="192"/>
+      <c r="AF9" s="192"/>
+      <c r="AG9" s="192"/>
+      <c r="AH9" s="192"/>
+      <c r="AI9" s="192"/>
+      <c r="AJ9" s="192"/>
+      <c r="AK9" s="192"/>
+      <c r="AL9" s="192"/>
+      <c r="AM9" s="192"/>
+      <c r="AN9" s="192"/>
+      <c r="AO9" s="192"/>
+      <c r="AP9" s="192"/>
+      <c r="AQ9" s="192"/>
+      <c r="AR9" s="192"/>
+      <c r="AS9" s="192"/>
+      <c r="AT9" s="192"/>
+      <c r="AU9" s="192"/>
+      <c r="AV9" s="192"/>
+      <c r="AW9" s="192"/>
+      <c r="AX9" s="192"/>
+      <c r="AY9" s="192"/>
+      <c r="AZ9" s="192"/>
+      <c r="BA9" s="192"/>
+      <c r="BB9" s="192"/>
+      <c r="BC9" s="192"/>
+      <c r="BD9" s="192"/>
+      <c r="BE9" s="192"/>
+      <c r="BF9" s="192"/>
+      <c r="BG9" s="193"/>
     </row>
     <row r="10" spans="2:59" ht="30" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="186" t="s">
+      <c r="B10" s="197" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="187"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="187"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="187"/>
-      <c r="H10" s="187"/>
-      <c r="I10" s="187"/>
-      <c r="J10" s="187"/>
-      <c r="K10" s="187"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="187"/>
-      <c r="X10" s="187"/>
-      <c r="Y10" s="210"/>
-      <c r="Z10" s="210"/>
-      <c r="AA10" s="210"/>
-      <c r="AB10" s="210"/>
-      <c r="AC10" s="210"/>
-      <c r="AD10" s="210"/>
-      <c r="AE10" s="210"/>
-      <c r="AF10" s="210"/>
-      <c r="AG10" s="210"/>
-      <c r="AH10" s="210"/>
-      <c r="AI10" s="210"/>
-      <c r="AJ10" s="210"/>
-      <c r="AK10" s="210"/>
-      <c r="AL10" s="210"/>
-      <c r="AM10" s="210"/>
-      <c r="AN10" s="210"/>
-      <c r="AO10" s="210"/>
-      <c r="AP10" s="210"/>
-      <c r="AQ10" s="210"/>
-      <c r="AR10" s="210"/>
-      <c r="AS10" s="210"/>
-      <c r="AT10" s="210"/>
-      <c r="AU10" s="210"/>
-      <c r="AV10" s="210"/>
-      <c r="AW10" s="210"/>
-      <c r="AX10" s="210"/>
-      <c r="AY10" s="210"/>
-      <c r="AZ10" s="210"/>
-      <c r="BA10" s="210"/>
-      <c r="BB10" s="210"/>
-      <c r="BC10" s="210"/>
-      <c r="BD10" s="210"/>
-      <c r="BE10" s="210"/>
-      <c r="BF10" s="210"/>
-      <c r="BG10" s="188"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="198"/>
+      <c r="E10" s="198"/>
+      <c r="F10" s="198"/>
+      <c r="G10" s="198"/>
+      <c r="H10" s="198"/>
+      <c r="I10" s="198"/>
+      <c r="J10" s="198"/>
+      <c r="K10" s="198"/>
+      <c r="L10" s="198"/>
+      <c r="M10" s="198"/>
+      <c r="N10" s="198"/>
+      <c r="O10" s="198"/>
+      <c r="P10" s="198"/>
+      <c r="Q10" s="198"/>
+      <c r="R10" s="198"/>
+      <c r="S10" s="198"/>
+      <c r="T10" s="198"/>
+      <c r="U10" s="198"/>
+      <c r="V10" s="198"/>
+      <c r="W10" s="198"/>
+      <c r="X10" s="198"/>
+      <c r="Y10" s="203"/>
+      <c r="Z10" s="203"/>
+      <c r="AA10" s="203"/>
+      <c r="AB10" s="203"/>
+      <c r="AC10" s="203"/>
+      <c r="AD10" s="203"/>
+      <c r="AE10" s="203"/>
+      <c r="AF10" s="203"/>
+      <c r="AG10" s="203"/>
+      <c r="AH10" s="203"/>
+      <c r="AI10" s="203"/>
+      <c r="AJ10" s="203"/>
+      <c r="AK10" s="203"/>
+      <c r="AL10" s="203"/>
+      <c r="AM10" s="203"/>
+      <c r="AN10" s="203"/>
+      <c r="AO10" s="203"/>
+      <c r="AP10" s="203"/>
+      <c r="AQ10" s="203"/>
+      <c r="AR10" s="203"/>
+      <c r="AS10" s="203"/>
+      <c r="AT10" s="203"/>
+      <c r="AU10" s="203"/>
+      <c r="AV10" s="203"/>
+      <c r="AW10" s="203"/>
+      <c r="AX10" s="203"/>
+      <c r="AY10" s="203"/>
+      <c r="AZ10" s="203"/>
+      <c r="BA10" s="203"/>
+      <c r="BB10" s="203"/>
+      <c r="BC10" s="203"/>
+      <c r="BD10" s="203"/>
+      <c r="BE10" s="203"/>
+      <c r="BF10" s="203"/>
+      <c r="BG10" s="199"/>
     </row>
     <row r="11" spans="2:59" ht="30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="64"/>
@@ -22722,84 +22722,84 @@
     </row>
     <row r="12" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="70"/>
-      <c r="C12" s="203" t="s">
+      <c r="C12" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="204"/>
-      <c r="E12" s="205"/>
-      <c r="F12" s="206"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="180"/>
+      <c r="F12" s="181"/>
       <c r="G12" s="71"/>
-      <c r="H12" s="207" t="s">
+      <c r="H12" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="204"/>
-      <c r="J12" s="205"/>
-      <c r="K12" s="205"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="180"/>
+      <c r="K12" s="180"/>
       <c r="L12" s="71"/>
-      <c r="M12" s="203" t="s">
+      <c r="M12" s="178" t="s">
         <v>49</v>
       </c>
-      <c r="N12" s="204"/>
-      <c r="O12" s="205"/>
-      <c r="P12" s="206"/>
-      <c r="Q12" s="203" t="s">
+      <c r="N12" s="179"/>
+      <c r="O12" s="180"/>
+      <c r="P12" s="181"/>
+      <c r="Q12" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="R12" s="204"/>
-      <c r="S12" s="205"/>
-      <c r="T12" s="206"/>
-      <c r="U12" s="203" t="s">
+      <c r="R12" s="179"/>
+      <c r="S12" s="180"/>
+      <c r="T12" s="181"/>
+      <c r="U12" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="V12" s="204"/>
-      <c r="W12" s="205"/>
-      <c r="X12" s="206"/>
+      <c r="V12" s="179"/>
+      <c r="W12" s="180"/>
+      <c r="X12" s="181"/>
       <c r="Y12" s="36"/>
-      <c r="Z12" s="178" t="s">
+      <c r="Z12" s="183" t="s">
         <v>52</v>
       </c>
-      <c r="AA12" s="179"/>
-      <c r="AB12" s="179"/>
-      <c r="AC12" s="180"/>
+      <c r="AA12" s="184"/>
+      <c r="AB12" s="184"/>
+      <c r="AC12" s="185"/>
       <c r="AD12" s="71"/>
-      <c r="AE12" s="179" t="s">
+      <c r="AE12" s="184" t="s">
         <v>53</v>
       </c>
-      <c r="AF12" s="179"/>
-      <c r="AG12" s="179"/>
-      <c r="AH12" s="179"/>
+      <c r="AF12" s="184"/>
+      <c r="AG12" s="184"/>
+      <c r="AH12" s="184"/>
       <c r="AI12" s="36"/>
-      <c r="AJ12" s="208" t="s">
+      <c r="AJ12" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="AK12" s="209"/>
-      <c r="AL12" s="209"/>
-      <c r="AM12" s="178" t="s">
+      <c r="AK12" s="187"/>
+      <c r="AL12" s="187"/>
+      <c r="AM12" s="183" t="s">
         <v>55</v>
       </c>
-      <c r="AN12" s="179"/>
-      <c r="AO12" s="179"/>
-      <c r="AP12" s="179"/>
-      <c r="AQ12" s="180"/>
-      <c r="AR12" s="181" t="s">
+      <c r="AN12" s="184"/>
+      <c r="AO12" s="184"/>
+      <c r="AP12" s="184"/>
+      <c r="AQ12" s="185"/>
+      <c r="AR12" s="175" t="s">
         <v>87</v>
       </c>
-      <c r="AS12" s="182"/>
-      <c r="AT12" s="182"/>
-      <c r="AU12" s="182"/>
-      <c r="AV12" s="183"/>
-      <c r="AW12" s="181" t="s">
+      <c r="AS12" s="176"/>
+      <c r="AT12" s="176"/>
+      <c r="AU12" s="176"/>
+      <c r="AV12" s="177"/>
+      <c r="AW12" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="AX12" s="182"/>
-      <c r="AY12" s="183"/>
+      <c r="AX12" s="176"/>
+      <c r="AY12" s="177"/>
       <c r="AZ12" s="37"/>
-      <c r="BA12" s="184" t="s">
+      <c r="BA12" s="209" t="s">
         <v>104</v>
       </c>
-      <c r="BB12" s="185"/>
-      <c r="BC12" s="185"/>
-      <c r="BD12" s="185"/>
+      <c r="BB12" s="210"/>
+      <c r="BC12" s="210"/>
+      <c r="BD12" s="210"/>
       <c r="BE12" s="38"/>
       <c r="BF12" s="72"/>
       <c r="BG12" s="73"/>
@@ -25850,66 +25850,66 @@
       <c r="BG29" s="118"/>
     </row>
     <row r="30" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="186" t="s">
+      <c r="B30" s="197" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="187"/>
-      <c r="D30" s="187"/>
-      <c r="E30" s="187"/>
-      <c r="F30" s="187"/>
-      <c r="G30" s="187"/>
-      <c r="H30" s="187"/>
-      <c r="I30" s="187"/>
-      <c r="J30" s="187"/>
-      <c r="K30" s="187"/>
-      <c r="L30" s="187"/>
-      <c r="M30" s="187"/>
-      <c r="N30" s="187"/>
-      <c r="O30" s="187"/>
-      <c r="P30" s="187"/>
-      <c r="Q30" s="187"/>
-      <c r="R30" s="187"/>
-      <c r="S30" s="187"/>
-      <c r="T30" s="187"/>
-      <c r="U30" s="187"/>
-      <c r="V30" s="187"/>
-      <c r="W30" s="187"/>
-      <c r="X30" s="187"/>
-      <c r="Y30" s="187"/>
-      <c r="Z30" s="187"/>
-      <c r="AA30" s="187"/>
-      <c r="AB30" s="187"/>
-      <c r="AC30" s="187"/>
-      <c r="AD30" s="187"/>
-      <c r="AE30" s="187"/>
-      <c r="AF30" s="187"/>
-      <c r="AG30" s="187"/>
-      <c r="AH30" s="187"/>
-      <c r="AI30" s="187"/>
-      <c r="AJ30" s="187"/>
-      <c r="AK30" s="187"/>
-      <c r="AL30" s="187"/>
-      <c r="AM30" s="187"/>
-      <c r="AN30" s="187"/>
-      <c r="AO30" s="187"/>
-      <c r="AP30" s="187"/>
-      <c r="AQ30" s="187"/>
-      <c r="AR30" s="187"/>
-      <c r="AS30" s="187"/>
-      <c r="AT30" s="187"/>
-      <c r="AU30" s="187"/>
-      <c r="AV30" s="187"/>
-      <c r="AW30" s="187"/>
-      <c r="AX30" s="187"/>
-      <c r="AY30" s="187"/>
-      <c r="AZ30" s="187"/>
-      <c r="BA30" s="187"/>
-      <c r="BB30" s="187"/>
-      <c r="BC30" s="187"/>
-      <c r="BD30" s="187"/>
-      <c r="BE30" s="187"/>
-      <c r="BF30" s="187"/>
-      <c r="BG30" s="188"/>
+      <c r="C30" s="198"/>
+      <c r="D30" s="198"/>
+      <c r="E30" s="198"/>
+      <c r="F30" s="198"/>
+      <c r="G30" s="198"/>
+      <c r="H30" s="198"/>
+      <c r="I30" s="198"/>
+      <c r="J30" s="198"/>
+      <c r="K30" s="198"/>
+      <c r="L30" s="198"/>
+      <c r="M30" s="198"/>
+      <c r="N30" s="198"/>
+      <c r="O30" s="198"/>
+      <c r="P30" s="198"/>
+      <c r="Q30" s="198"/>
+      <c r="R30" s="198"/>
+      <c r="S30" s="198"/>
+      <c r="T30" s="198"/>
+      <c r="U30" s="198"/>
+      <c r="V30" s="198"/>
+      <c r="W30" s="198"/>
+      <c r="X30" s="198"/>
+      <c r="Y30" s="198"/>
+      <c r="Z30" s="198"/>
+      <c r="AA30" s="198"/>
+      <c r="AB30" s="198"/>
+      <c r="AC30" s="198"/>
+      <c r="AD30" s="198"/>
+      <c r="AE30" s="198"/>
+      <c r="AF30" s="198"/>
+      <c r="AG30" s="198"/>
+      <c r="AH30" s="198"/>
+      <c r="AI30" s="198"/>
+      <c r="AJ30" s="198"/>
+      <c r="AK30" s="198"/>
+      <c r="AL30" s="198"/>
+      <c r="AM30" s="198"/>
+      <c r="AN30" s="198"/>
+      <c r="AO30" s="198"/>
+      <c r="AP30" s="198"/>
+      <c r="AQ30" s="198"/>
+      <c r="AR30" s="198"/>
+      <c r="AS30" s="198"/>
+      <c r="AT30" s="198"/>
+      <c r="AU30" s="198"/>
+      <c r="AV30" s="198"/>
+      <c r="AW30" s="198"/>
+      <c r="AX30" s="198"/>
+      <c r="AY30" s="198"/>
+      <c r="AZ30" s="198"/>
+      <c r="BA30" s="198"/>
+      <c r="BB30" s="198"/>
+      <c r="BC30" s="198"/>
+      <c r="BD30" s="198"/>
+      <c r="BE30" s="198"/>
+      <c r="BF30" s="198"/>
+      <c r="BG30" s="199"/>
     </row>
     <row r="31" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="80">
@@ -28797,66 +28797,66 @@
       <c r="BG46" s="141"/>
     </row>
     <row r="47" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="197" t="s">
+      <c r="B47" s="194" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="198"/>
-      <c r="D47" s="198"/>
-      <c r="E47" s="198"/>
-      <c r="F47" s="198"/>
-      <c r="G47" s="198"/>
-      <c r="H47" s="198"/>
-      <c r="I47" s="198"/>
-      <c r="J47" s="198"/>
-      <c r="K47" s="198"/>
-      <c r="L47" s="198"/>
-      <c r="M47" s="198"/>
-      <c r="N47" s="198"/>
-      <c r="O47" s="198"/>
-      <c r="P47" s="198"/>
-      <c r="Q47" s="198"/>
-      <c r="R47" s="198"/>
-      <c r="S47" s="198"/>
-      <c r="T47" s="198"/>
-      <c r="U47" s="198"/>
-      <c r="V47" s="198"/>
-      <c r="W47" s="198"/>
-      <c r="X47" s="198"/>
-      <c r="Y47" s="198"/>
-      <c r="Z47" s="198"/>
-      <c r="AA47" s="198"/>
-      <c r="AB47" s="198"/>
-      <c r="AC47" s="198"/>
-      <c r="AD47" s="198"/>
-      <c r="AE47" s="198"/>
-      <c r="AF47" s="198"/>
-      <c r="AG47" s="198"/>
-      <c r="AH47" s="198"/>
-      <c r="AI47" s="198"/>
-      <c r="AJ47" s="198"/>
-      <c r="AK47" s="198"/>
-      <c r="AL47" s="198"/>
-      <c r="AM47" s="198"/>
-      <c r="AN47" s="198"/>
-      <c r="AO47" s="198"/>
-      <c r="AP47" s="198"/>
-      <c r="AQ47" s="198"/>
-      <c r="AR47" s="198"/>
-      <c r="AS47" s="198"/>
-      <c r="AT47" s="198"/>
-      <c r="AU47" s="198"/>
-      <c r="AV47" s="198"/>
-      <c r="AW47" s="198"/>
-      <c r="AX47" s="198"/>
-      <c r="AY47" s="198"/>
-      <c r="AZ47" s="198"/>
-      <c r="BA47" s="198"/>
-      <c r="BB47" s="198"/>
-      <c r="BC47" s="198"/>
-      <c r="BD47" s="198"/>
-      <c r="BE47" s="198"/>
-      <c r="BF47" s="198"/>
-      <c r="BG47" s="199"/>
+      <c r="C47" s="195"/>
+      <c r="D47" s="195"/>
+      <c r="E47" s="195"/>
+      <c r="F47" s="195"/>
+      <c r="G47" s="195"/>
+      <c r="H47" s="195"/>
+      <c r="I47" s="195"/>
+      <c r="J47" s="195"/>
+      <c r="K47" s="195"/>
+      <c r="L47" s="195"/>
+      <c r="M47" s="195"/>
+      <c r="N47" s="195"/>
+      <c r="O47" s="195"/>
+      <c r="P47" s="195"/>
+      <c r="Q47" s="195"/>
+      <c r="R47" s="195"/>
+      <c r="S47" s="195"/>
+      <c r="T47" s="195"/>
+      <c r="U47" s="195"/>
+      <c r="V47" s="195"/>
+      <c r="W47" s="195"/>
+      <c r="X47" s="195"/>
+      <c r="Y47" s="195"/>
+      <c r="Z47" s="195"/>
+      <c r="AA47" s="195"/>
+      <c r="AB47" s="195"/>
+      <c r="AC47" s="195"/>
+      <c r="AD47" s="195"/>
+      <c r="AE47" s="195"/>
+      <c r="AF47" s="195"/>
+      <c r="AG47" s="195"/>
+      <c r="AH47" s="195"/>
+      <c r="AI47" s="195"/>
+      <c r="AJ47" s="195"/>
+      <c r="AK47" s="195"/>
+      <c r="AL47" s="195"/>
+      <c r="AM47" s="195"/>
+      <c r="AN47" s="195"/>
+      <c r="AO47" s="195"/>
+      <c r="AP47" s="195"/>
+      <c r="AQ47" s="195"/>
+      <c r="AR47" s="195"/>
+      <c r="AS47" s="195"/>
+      <c r="AT47" s="195"/>
+      <c r="AU47" s="195"/>
+      <c r="AV47" s="195"/>
+      <c r="AW47" s="195"/>
+      <c r="AX47" s="195"/>
+      <c r="AY47" s="195"/>
+      <c r="AZ47" s="195"/>
+      <c r="BA47" s="195"/>
+      <c r="BB47" s="195"/>
+      <c r="BC47" s="195"/>
+      <c r="BD47" s="195"/>
+      <c r="BE47" s="195"/>
+      <c r="BF47" s="195"/>
+      <c r="BG47" s="196"/>
     </row>
     <row r="48" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B48" s="80">
@@ -29041,7 +29041,7 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG48" s="189"/>
+      <c r="BG48" s="211"/>
     </row>
     <row r="49" spans="2:59" s="101" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B49" s="95">
@@ -29215,7 +29215,7 @@
         <f t="shared" si="28"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG49" s="190"/>
+      <c r="BG49" s="212"/>
     </row>
     <row r="50" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B50" s="80">
@@ -31654,66 +31654,66 @@
       <c r="BG63" s="118"/>
     </row>
     <row r="64" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="186" t="s">
+      <c r="B64" s="197" t="s">
         <v>94</v>
       </c>
-      <c r="C64" s="187"/>
-      <c r="D64" s="187"/>
-      <c r="E64" s="187"/>
-      <c r="F64" s="187"/>
-      <c r="G64" s="187"/>
-      <c r="H64" s="187"/>
-      <c r="I64" s="187"/>
-      <c r="J64" s="187"/>
-      <c r="K64" s="187"/>
-      <c r="L64" s="187"/>
-      <c r="M64" s="187"/>
-      <c r="N64" s="187"/>
-      <c r="O64" s="187"/>
-      <c r="P64" s="187"/>
-      <c r="Q64" s="187"/>
-      <c r="R64" s="187"/>
-      <c r="S64" s="187"/>
-      <c r="T64" s="187"/>
-      <c r="U64" s="187"/>
-      <c r="V64" s="187"/>
-      <c r="W64" s="187"/>
-      <c r="X64" s="187"/>
-      <c r="Y64" s="187"/>
-      <c r="Z64" s="187"/>
-      <c r="AA64" s="187"/>
-      <c r="AB64" s="187"/>
-      <c r="AC64" s="187"/>
-      <c r="AD64" s="187"/>
-      <c r="AE64" s="187"/>
-      <c r="AF64" s="187"/>
-      <c r="AG64" s="187"/>
-      <c r="AH64" s="187"/>
-      <c r="AI64" s="187"/>
-      <c r="AJ64" s="187"/>
-      <c r="AK64" s="187"/>
-      <c r="AL64" s="187"/>
-      <c r="AM64" s="187"/>
-      <c r="AN64" s="187"/>
-      <c r="AO64" s="187"/>
-      <c r="AP64" s="187"/>
-      <c r="AQ64" s="187"/>
-      <c r="AR64" s="187"/>
-      <c r="AS64" s="187"/>
-      <c r="AT64" s="187"/>
-      <c r="AU64" s="187"/>
-      <c r="AV64" s="187"/>
-      <c r="AW64" s="187"/>
-      <c r="AX64" s="187"/>
-      <c r="AY64" s="187"/>
-      <c r="AZ64" s="187"/>
-      <c r="BA64" s="187"/>
-      <c r="BB64" s="187"/>
-      <c r="BC64" s="187"/>
-      <c r="BD64" s="187"/>
-      <c r="BE64" s="187"/>
-      <c r="BF64" s="187"/>
-      <c r="BG64" s="188"/>
+      <c r="C64" s="198"/>
+      <c r="D64" s="198"/>
+      <c r="E64" s="198"/>
+      <c r="F64" s="198"/>
+      <c r="G64" s="198"/>
+      <c r="H64" s="198"/>
+      <c r="I64" s="198"/>
+      <c r="J64" s="198"/>
+      <c r="K64" s="198"/>
+      <c r="L64" s="198"/>
+      <c r="M64" s="198"/>
+      <c r="N64" s="198"/>
+      <c r="O64" s="198"/>
+      <c r="P64" s="198"/>
+      <c r="Q64" s="198"/>
+      <c r="R64" s="198"/>
+      <c r="S64" s="198"/>
+      <c r="T64" s="198"/>
+      <c r="U64" s="198"/>
+      <c r="V64" s="198"/>
+      <c r="W64" s="198"/>
+      <c r="X64" s="198"/>
+      <c r="Y64" s="198"/>
+      <c r="Z64" s="198"/>
+      <c r="AA64" s="198"/>
+      <c r="AB64" s="198"/>
+      <c r="AC64" s="198"/>
+      <c r="AD64" s="198"/>
+      <c r="AE64" s="198"/>
+      <c r="AF64" s="198"/>
+      <c r="AG64" s="198"/>
+      <c r="AH64" s="198"/>
+      <c r="AI64" s="198"/>
+      <c r="AJ64" s="198"/>
+      <c r="AK64" s="198"/>
+      <c r="AL64" s="198"/>
+      <c r="AM64" s="198"/>
+      <c r="AN64" s="198"/>
+      <c r="AO64" s="198"/>
+      <c r="AP64" s="198"/>
+      <c r="AQ64" s="198"/>
+      <c r="AR64" s="198"/>
+      <c r="AS64" s="198"/>
+      <c r="AT64" s="198"/>
+      <c r="AU64" s="198"/>
+      <c r="AV64" s="198"/>
+      <c r="AW64" s="198"/>
+      <c r="AX64" s="198"/>
+      <c r="AY64" s="198"/>
+      <c r="AZ64" s="198"/>
+      <c r="BA64" s="198"/>
+      <c r="BB64" s="198"/>
+      <c r="BC64" s="198"/>
+      <c r="BD64" s="198"/>
+      <c r="BE64" s="198"/>
+      <c r="BF64" s="198"/>
+      <c r="BG64" s="199"/>
     </row>
     <row r="65" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B65" s="80">
@@ -34511,66 +34511,66 @@
       <c r="BG80" s="152"/>
     </row>
     <row r="81" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="186" t="s">
+      <c r="B81" s="197" t="s">
         <v>95</v>
       </c>
-      <c r="C81" s="187"/>
-      <c r="D81" s="187"/>
-      <c r="E81" s="187"/>
-      <c r="F81" s="187"/>
-      <c r="G81" s="187"/>
-      <c r="H81" s="187"/>
-      <c r="I81" s="187"/>
-      <c r="J81" s="187"/>
-      <c r="K81" s="187"/>
-      <c r="L81" s="187"/>
-      <c r="M81" s="187"/>
-      <c r="N81" s="187"/>
-      <c r="O81" s="187"/>
-      <c r="P81" s="187"/>
-      <c r="Q81" s="187"/>
-      <c r="R81" s="187"/>
-      <c r="S81" s="187"/>
-      <c r="T81" s="187"/>
-      <c r="U81" s="187"/>
-      <c r="V81" s="187"/>
-      <c r="W81" s="187"/>
-      <c r="X81" s="187"/>
-      <c r="Y81" s="187"/>
-      <c r="Z81" s="187"/>
-      <c r="AA81" s="187"/>
-      <c r="AB81" s="187"/>
-      <c r="AC81" s="187"/>
-      <c r="AD81" s="187"/>
-      <c r="AE81" s="187"/>
-      <c r="AF81" s="187"/>
-      <c r="AG81" s="187"/>
-      <c r="AH81" s="187"/>
-      <c r="AI81" s="187"/>
-      <c r="AJ81" s="187"/>
-      <c r="AK81" s="187"/>
-      <c r="AL81" s="187"/>
-      <c r="AM81" s="187"/>
-      <c r="AN81" s="187"/>
-      <c r="AO81" s="187"/>
-      <c r="AP81" s="187"/>
-      <c r="AQ81" s="187"/>
-      <c r="AR81" s="187"/>
-      <c r="AS81" s="187"/>
-      <c r="AT81" s="187"/>
-      <c r="AU81" s="187"/>
-      <c r="AV81" s="187"/>
-      <c r="AW81" s="187"/>
-      <c r="AX81" s="187"/>
-      <c r="AY81" s="187"/>
-      <c r="AZ81" s="187"/>
-      <c r="BA81" s="187"/>
-      <c r="BB81" s="187"/>
-      <c r="BC81" s="187"/>
-      <c r="BD81" s="187"/>
-      <c r="BE81" s="187"/>
-      <c r="BF81" s="187"/>
-      <c r="BG81" s="188"/>
+      <c r="C81" s="198"/>
+      <c r="D81" s="198"/>
+      <c r="E81" s="198"/>
+      <c r="F81" s="198"/>
+      <c r="G81" s="198"/>
+      <c r="H81" s="198"/>
+      <c r="I81" s="198"/>
+      <c r="J81" s="198"/>
+      <c r="K81" s="198"/>
+      <c r="L81" s="198"/>
+      <c r="M81" s="198"/>
+      <c r="N81" s="198"/>
+      <c r="O81" s="198"/>
+      <c r="P81" s="198"/>
+      <c r="Q81" s="198"/>
+      <c r="R81" s="198"/>
+      <c r="S81" s="198"/>
+      <c r="T81" s="198"/>
+      <c r="U81" s="198"/>
+      <c r="V81" s="198"/>
+      <c r="W81" s="198"/>
+      <c r="X81" s="198"/>
+      <c r="Y81" s="198"/>
+      <c r="Z81" s="198"/>
+      <c r="AA81" s="198"/>
+      <c r="AB81" s="198"/>
+      <c r="AC81" s="198"/>
+      <c r="AD81" s="198"/>
+      <c r="AE81" s="198"/>
+      <c r="AF81" s="198"/>
+      <c r="AG81" s="198"/>
+      <c r="AH81" s="198"/>
+      <c r="AI81" s="198"/>
+      <c r="AJ81" s="198"/>
+      <c r="AK81" s="198"/>
+      <c r="AL81" s="198"/>
+      <c r="AM81" s="198"/>
+      <c r="AN81" s="198"/>
+      <c r="AO81" s="198"/>
+      <c r="AP81" s="198"/>
+      <c r="AQ81" s="198"/>
+      <c r="AR81" s="198"/>
+      <c r="AS81" s="198"/>
+      <c r="AT81" s="198"/>
+      <c r="AU81" s="198"/>
+      <c r="AV81" s="198"/>
+      <c r="AW81" s="198"/>
+      <c r="AX81" s="198"/>
+      <c r="AY81" s="198"/>
+      <c r="AZ81" s="198"/>
+      <c r="BA81" s="198"/>
+      <c r="BB81" s="198"/>
+      <c r="BC81" s="198"/>
+      <c r="BD81" s="198"/>
+      <c r="BE81" s="198"/>
+      <c r="BF81" s="198"/>
+      <c r="BG81" s="199"/>
     </row>
     <row r="82" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B82" s="80">
@@ -34761,7 +34761,7 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG82" s="173"/>
+      <c r="BG82" s="204"/>
     </row>
     <row r="83" spans="2:59" s="101" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B83" s="95">
@@ -34941,7 +34941,7 @@
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG83" s="174"/>
+      <c r="BG83" s="205"/>
     </row>
     <row r="84" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B84" s="80">
@@ -37464,66 +37464,66 @@
       <c r="BG97" s="152"/>
     </row>
     <row r="98" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B98" s="186" t="s">
+      <c r="B98" s="197" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="187"/>
-      <c r="D98" s="187"/>
-      <c r="E98" s="187"/>
-      <c r="F98" s="187"/>
-      <c r="G98" s="187"/>
-      <c r="H98" s="187"/>
-      <c r="I98" s="187"/>
-      <c r="J98" s="187"/>
-      <c r="K98" s="187"/>
-      <c r="L98" s="187"/>
-      <c r="M98" s="187"/>
-      <c r="N98" s="187"/>
-      <c r="O98" s="187"/>
-      <c r="P98" s="187"/>
-      <c r="Q98" s="187"/>
-      <c r="R98" s="187"/>
-      <c r="S98" s="187"/>
-      <c r="T98" s="187"/>
-      <c r="U98" s="187"/>
-      <c r="V98" s="187"/>
-      <c r="W98" s="187"/>
-      <c r="X98" s="187"/>
-      <c r="Y98" s="187"/>
-      <c r="Z98" s="187"/>
-      <c r="AA98" s="187"/>
-      <c r="AB98" s="187"/>
-      <c r="AC98" s="187"/>
-      <c r="AD98" s="187"/>
-      <c r="AE98" s="187"/>
-      <c r="AF98" s="187"/>
-      <c r="AG98" s="187"/>
-      <c r="AH98" s="187"/>
-      <c r="AI98" s="187"/>
-      <c r="AJ98" s="187"/>
-      <c r="AK98" s="187"/>
-      <c r="AL98" s="187"/>
-      <c r="AM98" s="187"/>
-      <c r="AN98" s="187"/>
-      <c r="AO98" s="187"/>
-      <c r="AP98" s="187"/>
-      <c r="AQ98" s="187"/>
-      <c r="AR98" s="187"/>
-      <c r="AS98" s="187"/>
-      <c r="AT98" s="187"/>
-      <c r="AU98" s="187"/>
-      <c r="AV98" s="187"/>
-      <c r="AW98" s="187"/>
-      <c r="AX98" s="187"/>
-      <c r="AY98" s="187"/>
-      <c r="AZ98" s="187"/>
-      <c r="BA98" s="187"/>
-      <c r="BB98" s="187"/>
-      <c r="BC98" s="187"/>
-      <c r="BD98" s="187"/>
-      <c r="BE98" s="187"/>
-      <c r="BF98" s="187"/>
-      <c r="BG98" s="188"/>
+      <c r="C98" s="198"/>
+      <c r="D98" s="198"/>
+      <c r="E98" s="198"/>
+      <c r="F98" s="198"/>
+      <c r="G98" s="198"/>
+      <c r="H98" s="198"/>
+      <c r="I98" s="198"/>
+      <c r="J98" s="198"/>
+      <c r="K98" s="198"/>
+      <c r="L98" s="198"/>
+      <c r="M98" s="198"/>
+      <c r="N98" s="198"/>
+      <c r="O98" s="198"/>
+      <c r="P98" s="198"/>
+      <c r="Q98" s="198"/>
+      <c r="R98" s="198"/>
+      <c r="S98" s="198"/>
+      <c r="T98" s="198"/>
+      <c r="U98" s="198"/>
+      <c r="V98" s="198"/>
+      <c r="W98" s="198"/>
+      <c r="X98" s="198"/>
+      <c r="Y98" s="198"/>
+      <c r="Z98" s="198"/>
+      <c r="AA98" s="198"/>
+      <c r="AB98" s="198"/>
+      <c r="AC98" s="198"/>
+      <c r="AD98" s="198"/>
+      <c r="AE98" s="198"/>
+      <c r="AF98" s="198"/>
+      <c r="AG98" s="198"/>
+      <c r="AH98" s="198"/>
+      <c r="AI98" s="198"/>
+      <c r="AJ98" s="198"/>
+      <c r="AK98" s="198"/>
+      <c r="AL98" s="198"/>
+      <c r="AM98" s="198"/>
+      <c r="AN98" s="198"/>
+      <c r="AO98" s="198"/>
+      <c r="AP98" s="198"/>
+      <c r="AQ98" s="198"/>
+      <c r="AR98" s="198"/>
+      <c r="AS98" s="198"/>
+      <c r="AT98" s="198"/>
+      <c r="AU98" s="198"/>
+      <c r="AV98" s="198"/>
+      <c r="AW98" s="198"/>
+      <c r="AX98" s="198"/>
+      <c r="AY98" s="198"/>
+      <c r="AZ98" s="198"/>
+      <c r="BA98" s="198"/>
+      <c r="BB98" s="198"/>
+      <c r="BC98" s="198"/>
+      <c r="BD98" s="198"/>
+      <c r="BE98" s="198"/>
+      <c r="BF98" s="198"/>
+      <c r="BG98" s="199"/>
     </row>
     <row r="99" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B99" s="80">
@@ -37714,7 +37714,7 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG99" s="173"/>
+      <c r="BG99" s="204"/>
     </row>
     <row r="100" spans="2:59" s="101" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B100" s="95">
@@ -37894,7 +37894,7 @@
         <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG100" s="174"/>
+      <c r="BG100" s="205"/>
     </row>
     <row r="101" spans="2:59" s="94" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B101" s="80">
@@ -40417,66 +40417,66 @@
       <c r="BG114" s="118"/>
     </row>
     <row r="115" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B115" s="186" t="s">
+      <c r="B115" s="197" t="s">
         <v>97</v>
       </c>
-      <c r="C115" s="187"/>
-      <c r="D115" s="187"/>
-      <c r="E115" s="187"/>
-      <c r="F115" s="187"/>
-      <c r="G115" s="187"/>
-      <c r="H115" s="187"/>
-      <c r="I115" s="187"/>
-      <c r="J115" s="187"/>
-      <c r="K115" s="187"/>
-      <c r="L115" s="187"/>
-      <c r="M115" s="187"/>
-      <c r="N115" s="187"/>
-      <c r="O115" s="187"/>
-      <c r="P115" s="187"/>
-      <c r="Q115" s="187"/>
-      <c r="R115" s="187"/>
-      <c r="S115" s="187"/>
-      <c r="T115" s="187"/>
-      <c r="U115" s="187"/>
-      <c r="V115" s="187"/>
-      <c r="W115" s="187"/>
-      <c r="X115" s="187"/>
-      <c r="Y115" s="187"/>
-      <c r="Z115" s="187"/>
-      <c r="AA115" s="187"/>
-      <c r="AB115" s="187"/>
-      <c r="AC115" s="187"/>
-      <c r="AD115" s="187"/>
-      <c r="AE115" s="187"/>
-      <c r="AF115" s="187"/>
-      <c r="AG115" s="187"/>
-      <c r="AH115" s="187"/>
-      <c r="AI115" s="187"/>
-      <c r="AJ115" s="187"/>
-      <c r="AK115" s="187"/>
-      <c r="AL115" s="187"/>
-      <c r="AM115" s="187"/>
-      <c r="AN115" s="187"/>
-      <c r="AO115" s="187"/>
-      <c r="AP115" s="187"/>
-      <c r="AQ115" s="187"/>
-      <c r="AR115" s="187"/>
-      <c r="AS115" s="187"/>
-      <c r="AT115" s="187"/>
-      <c r="AU115" s="187"/>
-      <c r="AV115" s="187"/>
-      <c r="AW115" s="187"/>
-      <c r="AX115" s="187"/>
-      <c r="AY115" s="187"/>
-      <c r="AZ115" s="187"/>
-      <c r="BA115" s="187"/>
-      <c r="BB115" s="187"/>
-      <c r="BC115" s="187"/>
-      <c r="BD115" s="187"/>
-      <c r="BE115" s="187"/>
-      <c r="BF115" s="187"/>
-      <c r="BG115" s="188"/>
+      <c r="C115" s="198"/>
+      <c r="D115" s="198"/>
+      <c r="E115" s="198"/>
+      <c r="F115" s="198"/>
+      <c r="G115" s="198"/>
+      <c r="H115" s="198"/>
+      <c r="I115" s="198"/>
+      <c r="J115" s="198"/>
+      <c r="K115" s="198"/>
+      <c r="L115" s="198"/>
+      <c r="M115" s="198"/>
+      <c r="N115" s="198"/>
+      <c r="O115" s="198"/>
+      <c r="P115" s="198"/>
+      <c r="Q115" s="198"/>
+      <c r="R115" s="198"/>
+      <c r="S115" s="198"/>
+      <c r="T115" s="198"/>
+      <c r="U115" s="198"/>
+      <c r="V115" s="198"/>
+      <c r="W115" s="198"/>
+      <c r="X115" s="198"/>
+      <c r="Y115" s="198"/>
+      <c r="Z115" s="198"/>
+      <c r="AA115" s="198"/>
+      <c r="AB115" s="198"/>
+      <c r="AC115" s="198"/>
+      <c r="AD115" s="198"/>
+      <c r="AE115" s="198"/>
+      <c r="AF115" s="198"/>
+      <c r="AG115" s="198"/>
+      <c r="AH115" s="198"/>
+      <c r="AI115" s="198"/>
+      <c r="AJ115" s="198"/>
+      <c r="AK115" s="198"/>
+      <c r="AL115" s="198"/>
+      <c r="AM115" s="198"/>
+      <c r="AN115" s="198"/>
+      <c r="AO115" s="198"/>
+      <c r="AP115" s="198"/>
+      <c r="AQ115" s="198"/>
+      <c r="AR115" s="198"/>
+      <c r="AS115" s="198"/>
+      <c r="AT115" s="198"/>
+      <c r="AU115" s="198"/>
+      <c r="AV115" s="198"/>
+      <c r="AW115" s="198"/>
+      <c r="AX115" s="198"/>
+      <c r="AY115" s="198"/>
+      <c r="AZ115" s="198"/>
+      <c r="BA115" s="198"/>
+      <c r="BB115" s="198"/>
+      <c r="BC115" s="198"/>
+      <c r="BD115" s="198"/>
+      <c r="BE115" s="198"/>
+      <c r="BF115" s="198"/>
+      <c r="BG115" s="199"/>
     </row>
     <row r="116" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="80">
@@ -43370,66 +43370,66 @@
       <c r="BG131" s="152"/>
     </row>
     <row r="132" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="186" t="s">
+      <c r="B132" s="197" t="s">
         <v>99</v>
       </c>
-      <c r="C132" s="187"/>
-      <c r="D132" s="187"/>
-      <c r="E132" s="187"/>
-      <c r="F132" s="187"/>
-      <c r="G132" s="187"/>
-      <c r="H132" s="187"/>
-      <c r="I132" s="187"/>
-      <c r="J132" s="187"/>
-      <c r="K132" s="187"/>
-      <c r="L132" s="187"/>
-      <c r="M132" s="187"/>
-      <c r="N132" s="187"/>
-      <c r="O132" s="187"/>
-      <c r="P132" s="187"/>
-      <c r="Q132" s="187"/>
-      <c r="R132" s="187"/>
-      <c r="S132" s="187"/>
-      <c r="T132" s="187"/>
-      <c r="U132" s="187"/>
-      <c r="V132" s="187"/>
-      <c r="W132" s="187"/>
-      <c r="X132" s="187"/>
-      <c r="Y132" s="187"/>
-      <c r="Z132" s="187"/>
-      <c r="AA132" s="187"/>
-      <c r="AB132" s="187"/>
-      <c r="AC132" s="187"/>
-      <c r="AD132" s="187"/>
-      <c r="AE132" s="187"/>
-      <c r="AF132" s="187"/>
-      <c r="AG132" s="187"/>
-      <c r="AH132" s="187"/>
-      <c r="AI132" s="187"/>
-      <c r="AJ132" s="187"/>
-      <c r="AK132" s="187"/>
-      <c r="AL132" s="187"/>
-      <c r="AM132" s="187"/>
-      <c r="AN132" s="187"/>
-      <c r="AO132" s="187"/>
-      <c r="AP132" s="187"/>
-      <c r="AQ132" s="187"/>
-      <c r="AR132" s="187"/>
-      <c r="AS132" s="187"/>
-      <c r="AT132" s="187"/>
-      <c r="AU132" s="187"/>
-      <c r="AV132" s="187"/>
-      <c r="AW132" s="187"/>
-      <c r="AX132" s="187"/>
-      <c r="AY132" s="187"/>
-      <c r="AZ132" s="187"/>
-      <c r="BA132" s="187"/>
-      <c r="BB132" s="187"/>
-      <c r="BC132" s="187"/>
-      <c r="BD132" s="187"/>
-      <c r="BE132" s="187"/>
-      <c r="BF132" s="187"/>
-      <c r="BG132" s="188"/>
+      <c r="C132" s="198"/>
+      <c r="D132" s="198"/>
+      <c r="E132" s="198"/>
+      <c r="F132" s="198"/>
+      <c r="G132" s="198"/>
+      <c r="H132" s="198"/>
+      <c r="I132" s="198"/>
+      <c r="J132" s="198"/>
+      <c r="K132" s="198"/>
+      <c r="L132" s="198"/>
+      <c r="M132" s="198"/>
+      <c r="N132" s="198"/>
+      <c r="O132" s="198"/>
+      <c r="P132" s="198"/>
+      <c r="Q132" s="198"/>
+      <c r="R132" s="198"/>
+      <c r="S132" s="198"/>
+      <c r="T132" s="198"/>
+      <c r="U132" s="198"/>
+      <c r="V132" s="198"/>
+      <c r="W132" s="198"/>
+      <c r="X132" s="198"/>
+      <c r="Y132" s="198"/>
+      <c r="Z132" s="198"/>
+      <c r="AA132" s="198"/>
+      <c r="AB132" s="198"/>
+      <c r="AC132" s="198"/>
+      <c r="AD132" s="198"/>
+      <c r="AE132" s="198"/>
+      <c r="AF132" s="198"/>
+      <c r="AG132" s="198"/>
+      <c r="AH132" s="198"/>
+      <c r="AI132" s="198"/>
+      <c r="AJ132" s="198"/>
+      <c r="AK132" s="198"/>
+      <c r="AL132" s="198"/>
+      <c r="AM132" s="198"/>
+      <c r="AN132" s="198"/>
+      <c r="AO132" s="198"/>
+      <c r="AP132" s="198"/>
+      <c r="AQ132" s="198"/>
+      <c r="AR132" s="198"/>
+      <c r="AS132" s="198"/>
+      <c r="AT132" s="198"/>
+      <c r="AU132" s="198"/>
+      <c r="AV132" s="198"/>
+      <c r="AW132" s="198"/>
+      <c r="AX132" s="198"/>
+      <c r="AY132" s="198"/>
+      <c r="AZ132" s="198"/>
+      <c r="BA132" s="198"/>
+      <c r="BB132" s="198"/>
+      <c r="BC132" s="198"/>
+      <c r="BD132" s="198"/>
+      <c r="BE132" s="198"/>
+      <c r="BF132" s="198"/>
+      <c r="BG132" s="199"/>
     </row>
     <row r="133" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B133" s="80">
@@ -46355,66 +46355,66 @@
       <c r="BG148" s="152"/>
     </row>
     <row r="149" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B149" s="186" t="s">
+      <c r="B149" s="197" t="s">
         <v>100</v>
       </c>
-      <c r="C149" s="187"/>
-      <c r="D149" s="187"/>
-      <c r="E149" s="187"/>
-      <c r="F149" s="187"/>
-      <c r="G149" s="187"/>
-      <c r="H149" s="187"/>
-      <c r="I149" s="187"/>
-      <c r="J149" s="187"/>
-      <c r="K149" s="187"/>
-      <c r="L149" s="187"/>
-      <c r="M149" s="187"/>
-      <c r="N149" s="187"/>
-      <c r="O149" s="187"/>
-      <c r="P149" s="187"/>
-      <c r="Q149" s="187"/>
-      <c r="R149" s="187"/>
-      <c r="S149" s="187"/>
-      <c r="T149" s="187"/>
-      <c r="U149" s="187"/>
-      <c r="V149" s="187"/>
-      <c r="W149" s="187"/>
-      <c r="X149" s="187"/>
-      <c r="Y149" s="187"/>
-      <c r="Z149" s="187"/>
-      <c r="AA149" s="187"/>
-      <c r="AB149" s="187"/>
-      <c r="AC149" s="187"/>
-      <c r="AD149" s="187"/>
-      <c r="AE149" s="187"/>
-      <c r="AF149" s="187"/>
-      <c r="AG149" s="187"/>
-      <c r="AH149" s="187"/>
-      <c r="AI149" s="187"/>
-      <c r="AJ149" s="187"/>
-      <c r="AK149" s="187"/>
-      <c r="AL149" s="187"/>
-      <c r="AM149" s="187"/>
-      <c r="AN149" s="187"/>
-      <c r="AO149" s="187"/>
-      <c r="AP149" s="187"/>
-      <c r="AQ149" s="187"/>
-      <c r="AR149" s="187"/>
-      <c r="AS149" s="187"/>
-      <c r="AT149" s="187"/>
-      <c r="AU149" s="187"/>
-      <c r="AV149" s="187"/>
-      <c r="AW149" s="187"/>
-      <c r="AX149" s="187"/>
-      <c r="AY149" s="187"/>
-      <c r="AZ149" s="187"/>
-      <c r="BA149" s="187"/>
-      <c r="BB149" s="187"/>
-      <c r="BC149" s="187"/>
-      <c r="BD149" s="187"/>
-      <c r="BE149" s="187"/>
-      <c r="BF149" s="187"/>
-      <c r="BG149" s="188"/>
+      <c r="C149" s="198"/>
+      <c r="D149" s="198"/>
+      <c r="E149" s="198"/>
+      <c r="F149" s="198"/>
+      <c r="G149" s="198"/>
+      <c r="H149" s="198"/>
+      <c r="I149" s="198"/>
+      <c r="J149" s="198"/>
+      <c r="K149" s="198"/>
+      <c r="L149" s="198"/>
+      <c r="M149" s="198"/>
+      <c r="N149" s="198"/>
+      <c r="O149" s="198"/>
+      <c r="P149" s="198"/>
+      <c r="Q149" s="198"/>
+      <c r="R149" s="198"/>
+      <c r="S149" s="198"/>
+      <c r="T149" s="198"/>
+      <c r="U149" s="198"/>
+      <c r="V149" s="198"/>
+      <c r="W149" s="198"/>
+      <c r="X149" s="198"/>
+      <c r="Y149" s="198"/>
+      <c r="Z149" s="198"/>
+      <c r="AA149" s="198"/>
+      <c r="AB149" s="198"/>
+      <c r="AC149" s="198"/>
+      <c r="AD149" s="198"/>
+      <c r="AE149" s="198"/>
+      <c r="AF149" s="198"/>
+      <c r="AG149" s="198"/>
+      <c r="AH149" s="198"/>
+      <c r="AI149" s="198"/>
+      <c r="AJ149" s="198"/>
+      <c r="AK149" s="198"/>
+      <c r="AL149" s="198"/>
+      <c r="AM149" s="198"/>
+      <c r="AN149" s="198"/>
+      <c r="AO149" s="198"/>
+      <c r="AP149" s="198"/>
+      <c r="AQ149" s="198"/>
+      <c r="AR149" s="198"/>
+      <c r="AS149" s="198"/>
+      <c r="AT149" s="198"/>
+      <c r="AU149" s="198"/>
+      <c r="AV149" s="198"/>
+      <c r="AW149" s="198"/>
+      <c r="AX149" s="198"/>
+      <c r="AY149" s="198"/>
+      <c r="AZ149" s="198"/>
+      <c r="BA149" s="198"/>
+      <c r="BB149" s="198"/>
+      <c r="BC149" s="198"/>
+      <c r="BD149" s="198"/>
+      <c r="BE149" s="198"/>
+      <c r="BF149" s="198"/>
+      <c r="BG149" s="199"/>
     </row>
     <row r="150" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="80">
@@ -46599,7 +46599,7 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG150" s="173"/>
+      <c r="BG150" s="204"/>
     </row>
     <row r="151" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B151" s="80">
@@ -46775,7 +46775,7 @@
         <f t="shared" si="87"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG151" s="174"/>
+      <c r="BG151" s="205"/>
     </row>
     <row r="152" spans="2:59" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B152" s="80">
@@ -49264,66 +49264,66 @@
       <c r="BG165" s="152"/>
     </row>
     <row r="166" spans="2:59" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B166" s="186" t="s">
+      <c r="B166" s="197" t="s">
         <v>102</v>
       </c>
-      <c r="C166" s="187"/>
-      <c r="D166" s="187"/>
-      <c r="E166" s="187"/>
-      <c r="F166" s="187"/>
-      <c r="G166" s="187"/>
-      <c r="H166" s="187"/>
-      <c r="I166" s="187"/>
-      <c r="J166" s="187"/>
-      <c r="K166" s="187"/>
-      <c r="L166" s="187"/>
-      <c r="M166" s="187"/>
-      <c r="N166" s="187"/>
-      <c r="O166" s="187"/>
-      <c r="P166" s="187"/>
-      <c r="Q166" s="187"/>
-      <c r="R166" s="187"/>
-      <c r="S166" s="187"/>
-      <c r="T166" s="187"/>
-      <c r="U166" s="187"/>
-      <c r="V166" s="187"/>
-      <c r="W166" s="187"/>
-      <c r="X166" s="187"/>
-      <c r="Y166" s="187"/>
-      <c r="Z166" s="187"/>
-      <c r="AA166" s="187"/>
-      <c r="AB166" s="187"/>
-      <c r="AC166" s="187"/>
-      <c r="AD166" s="187"/>
-      <c r="AE166" s="187"/>
-      <c r="AF166" s="187"/>
-      <c r="AG166" s="187"/>
-      <c r="AH166" s="187"/>
-      <c r="AI166" s="187"/>
-      <c r="AJ166" s="187"/>
-      <c r="AK166" s="187"/>
-      <c r="AL166" s="187"/>
-      <c r="AM166" s="187"/>
-      <c r="AN166" s="187"/>
-      <c r="AO166" s="187"/>
-      <c r="AP166" s="187"/>
-      <c r="AQ166" s="187"/>
-      <c r="AR166" s="187"/>
-      <c r="AS166" s="187"/>
-      <c r="AT166" s="187"/>
-      <c r="AU166" s="187"/>
-      <c r="AV166" s="187"/>
-      <c r="AW166" s="187"/>
-      <c r="AX166" s="187"/>
-      <c r="AY166" s="187"/>
-      <c r="AZ166" s="187"/>
-      <c r="BA166" s="187"/>
-      <c r="BB166" s="187"/>
-      <c r="BC166" s="187"/>
-      <c r="BD166" s="187"/>
-      <c r="BE166" s="187"/>
-      <c r="BF166" s="187"/>
-      <c r="BG166" s="188"/>
+      <c r="C166" s="198"/>
+      <c r="D166" s="198"/>
+      <c r="E166" s="198"/>
+      <c r="F166" s="198"/>
+      <c r="G166" s="198"/>
+      <c r="H166" s="198"/>
+      <c r="I166" s="198"/>
+      <c r="J166" s="198"/>
+      <c r="K166" s="198"/>
+      <c r="L166" s="198"/>
+      <c r="M166" s="198"/>
+      <c r="N166" s="198"/>
+      <c r="O166" s="198"/>
+      <c r="P166" s="198"/>
+      <c r="Q166" s="198"/>
+      <c r="R166" s="198"/>
+      <c r="S166" s="198"/>
+      <c r="T166" s="198"/>
+      <c r="U166" s="198"/>
+      <c r="V166" s="198"/>
+      <c r="W166" s="198"/>
+      <c r="X166" s="198"/>
+      <c r="Y166" s="198"/>
+      <c r="Z166" s="198"/>
+      <c r="AA166" s="198"/>
+      <c r="AB166" s="198"/>
+      <c r="AC166" s="198"/>
+      <c r="AD166" s="198"/>
+      <c r="AE166" s="198"/>
+      <c r="AF166" s="198"/>
+      <c r="AG166" s="198"/>
+      <c r="AH166" s="198"/>
+      <c r="AI166" s="198"/>
+      <c r="AJ166" s="198"/>
+      <c r="AK166" s="198"/>
+      <c r="AL166" s="198"/>
+      <c r="AM166" s="198"/>
+      <c r="AN166" s="198"/>
+      <c r="AO166" s="198"/>
+      <c r="AP166" s="198"/>
+      <c r="AQ166" s="198"/>
+      <c r="AR166" s="198"/>
+      <c r="AS166" s="198"/>
+      <c r="AT166" s="198"/>
+      <c r="AU166" s="198"/>
+      <c r="AV166" s="198"/>
+      <c r="AW166" s="198"/>
+      <c r="AX166" s="198"/>
+      <c r="AY166" s="198"/>
+      <c r="AZ166" s="198"/>
+      <c r="BA166" s="198"/>
+      <c r="BB166" s="198"/>
+      <c r="BC166" s="198"/>
+      <c r="BD166" s="198"/>
+      <c r="BE166" s="198"/>
+      <c r="BF166" s="198"/>
+      <c r="BG166" s="199"/>
     </row>
     <row r="167" spans="2:59" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B167" s="80">
@@ -49514,7 +49514,7 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG167" s="173"/>
+      <c r="BG167" s="204"/>
     </row>
     <row r="168" spans="2:59" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B168" s="80">
@@ -49694,7 +49694,7 @@
         <f t="shared" si="98"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BG168" s="174"/>
+      <c r="BG168" s="205"/>
     </row>
     <row r="169" spans="2:59" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B169" s="80">
@@ -52217,66 +52217,66 @@
       <c r="BG182" s="152"/>
     </row>
     <row r="183" spans="2:59" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B183" s="175" t="s">
+      <c r="B183" s="206" t="s">
         <v>103</v>
       </c>
-      <c r="C183" s="176"/>
-      <c r="D183" s="176"/>
-      <c r="E183" s="176"/>
-      <c r="F183" s="176"/>
-      <c r="G183" s="176"/>
-      <c r="H183" s="176"/>
-      <c r="I183" s="176"/>
-      <c r="J183" s="176"/>
-      <c r="K183" s="176"/>
-      <c r="L183" s="176"/>
-      <c r="M183" s="176"/>
-      <c r="N183" s="176"/>
-      <c r="O183" s="176"/>
-      <c r="P183" s="176"/>
-      <c r="Q183" s="176"/>
-      <c r="R183" s="176"/>
-      <c r="S183" s="176"/>
-      <c r="T183" s="176"/>
-      <c r="U183" s="176"/>
-      <c r="V183" s="176"/>
-      <c r="W183" s="176"/>
-      <c r="X183" s="176"/>
-      <c r="Y183" s="176"/>
-      <c r="Z183" s="176"/>
-      <c r="AA183" s="176"/>
-      <c r="AB183" s="176"/>
-      <c r="AC183" s="176"/>
-      <c r="AD183" s="176"/>
-      <c r="AE183" s="176"/>
-      <c r="AF183" s="176"/>
-      <c r="AG183" s="176"/>
-      <c r="AH183" s="176"/>
-      <c r="AI183" s="176"/>
-      <c r="AJ183" s="176"/>
-      <c r="AK183" s="176"/>
-      <c r="AL183" s="176"/>
-      <c r="AM183" s="176"/>
-      <c r="AN183" s="176"/>
-      <c r="AO183" s="176"/>
-      <c r="AP183" s="176"/>
-      <c r="AQ183" s="176"/>
-      <c r="AR183" s="176"/>
-      <c r="AS183" s="176"/>
-      <c r="AT183" s="176"/>
-      <c r="AU183" s="176"/>
-      <c r="AV183" s="176"/>
-      <c r="AW183" s="176"/>
-      <c r="AX183" s="176"/>
-      <c r="AY183" s="176"/>
-      <c r="AZ183" s="176"/>
-      <c r="BA183" s="176"/>
-      <c r="BB183" s="176"/>
-      <c r="BC183" s="176"/>
-      <c r="BD183" s="176"/>
-      <c r="BE183" s="176"/>
-      <c r="BF183" s="176"/>
-      <c r="BG183" s="177"/>
+      <c r="C183" s="207"/>
+      <c r="D183" s="207"/>
+      <c r="E183" s="207"/>
+      <c r="F183" s="207"/>
+      <c r="G183" s="207"/>
+      <c r="H183" s="207"/>
+      <c r="I183" s="207"/>
+      <c r="J183" s="207"/>
+      <c r="K183" s="207"/>
+      <c r="L183" s="207"/>
+      <c r="M183" s="207"/>
+      <c r="N183" s="207"/>
+      <c r="O183" s="207"/>
+      <c r="P183" s="207"/>
+      <c r="Q183" s="207"/>
+      <c r="R183" s="207"/>
+      <c r="S183" s="207"/>
+      <c r="T183" s="207"/>
+      <c r="U183" s="207"/>
+      <c r="V183" s="207"/>
+      <c r="W183" s="207"/>
+      <c r="X183" s="207"/>
+      <c r="Y183" s="207"/>
+      <c r="Z183" s="207"/>
+      <c r="AA183" s="207"/>
+      <c r="AB183" s="207"/>
+      <c r="AC183" s="207"/>
+      <c r="AD183" s="207"/>
+      <c r="AE183" s="207"/>
+      <c r="AF183" s="207"/>
+      <c r="AG183" s="207"/>
+      <c r="AH183" s="207"/>
+      <c r="AI183" s="207"/>
+      <c r="AJ183" s="207"/>
+      <c r="AK183" s="207"/>
+      <c r="AL183" s="207"/>
+      <c r="AM183" s="207"/>
+      <c r="AN183" s="207"/>
+      <c r="AO183" s="207"/>
+      <c r="AP183" s="207"/>
+      <c r="AQ183" s="207"/>
+      <c r="AR183" s="207"/>
+      <c r="AS183" s="207"/>
+      <c r="AT183" s="207"/>
+      <c r="AU183" s="207"/>
+      <c r="AV183" s="207"/>
+      <c r="AW183" s="207"/>
+      <c r="AX183" s="207"/>
+      <c r="AY183" s="207"/>
+      <c r="AZ183" s="207"/>
+      <c r="BA183" s="207"/>
+      <c r="BB183" s="207"/>
+      <c r="BC183" s="207"/>
+      <c r="BD183" s="207"/>
+      <c r="BE183" s="207"/>
+      <c r="BF183" s="207"/>
+      <c r="BG183" s="208"/>
     </row>
     <row r="184" spans="2:59" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B184" s="142"/>
@@ -52462,21 +52462,22 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="U8:X8"/>
-    <mergeCell ref="AM8:AP8"/>
-    <mergeCell ref="BA8:BB8"/>
-    <mergeCell ref="BA2:BC2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AR2:AU2"/>
-    <mergeCell ref="AW2:AY2"/>
+    <mergeCell ref="BG167:BG168"/>
+    <mergeCell ref="B183:BG183"/>
+    <mergeCell ref="AM12:AQ12"/>
+    <mergeCell ref="AR12:AV12"/>
+    <mergeCell ref="BA12:BD12"/>
+    <mergeCell ref="BG150:BG151"/>
+    <mergeCell ref="B166:BG166"/>
+    <mergeCell ref="B149:BG149"/>
+    <mergeCell ref="B132:BG132"/>
+    <mergeCell ref="BG99:BG100"/>
+    <mergeCell ref="B115:BG115"/>
+    <mergeCell ref="B98:BG98"/>
+    <mergeCell ref="BG82:BG83"/>
+    <mergeCell ref="B81:BG81"/>
+    <mergeCell ref="B64:BG64"/>
+    <mergeCell ref="BG48:BG49"/>
     <mergeCell ref="BE8:BF8"/>
     <mergeCell ref="B9:BG9"/>
     <mergeCell ref="B47:BG47"/>
@@ -52493,22 +52494,21 @@
     <mergeCell ref="AE12:AH12"/>
     <mergeCell ref="AJ12:AL12"/>
     <mergeCell ref="B10:BG10"/>
-    <mergeCell ref="BG167:BG168"/>
-    <mergeCell ref="B183:BG183"/>
-    <mergeCell ref="AM12:AQ12"/>
-    <mergeCell ref="AR12:AV12"/>
-    <mergeCell ref="BA12:BD12"/>
-    <mergeCell ref="BG150:BG151"/>
-    <mergeCell ref="B166:BG166"/>
-    <mergeCell ref="B149:BG149"/>
-    <mergeCell ref="B132:BG132"/>
-    <mergeCell ref="BG99:BG100"/>
-    <mergeCell ref="B115:BG115"/>
-    <mergeCell ref="B98:BG98"/>
-    <mergeCell ref="BG82:BG83"/>
-    <mergeCell ref="B81:BG81"/>
-    <mergeCell ref="B64:BG64"/>
-    <mergeCell ref="BG48:BG49"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="AM8:AP8"/>
+    <mergeCell ref="BA8:BB8"/>
+    <mergeCell ref="BA2:BC2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="AW2:AY2"/>
   </mergeCells>
   <conditionalFormatting sqref="C48:G63 C65:G80 AM31:AY46 AV133:AY148">
     <cfRule type="cellIs" dxfId="933" priority="920" stopIfTrue="1" operator="equal">

</xml_diff>